<commit_message>
a revisar para version final
</commit_message>
<xml_diff>
--- a/tdse-tp1_00-problem_approach.xlsx
+++ b/tdse-tp1_00-problem_approach.xlsx
@@ -1,19 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EQUIPO\Desktop\TDSEM\tdse_workspace_tp1\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" activeTab="1"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sensor" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="System" sheetId="2" r:id="rId5"/>
-    <sheet state="visible" name="Actuator" sheetId="3" r:id="rId6"/>
+    <sheet name="Sensor" sheetId="1" r:id="rId1"/>
+    <sheet name="System" sheetId="2" r:id="rId2"/>
+    <sheet name="Actuator" sheetId="3" r:id="rId3"/>
   </sheets>
-  <definedNames/>
   <calcPr/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <si>
     <t>Sensor Statechart - State Transition Table</t>
   </si>
@@ -97,6 +103,12 @@
   </si>
   <si>
     <t>raise EV_ACT_RAISE_BARRIER; sys_tick=TIME_BARRIER</t>
+  </si>
+  <si>
+    <t>EV_SYS_01_RELEASED</t>
+  </si>
+  <si>
+    <t>(abortar proceso)</t>
   </si>
   <si>
     <t>EV_SYS_TICK</t>
@@ -186,38 +198,38 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="6">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
     </font>
-    <font/>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
     <font>
       <b/>
-      <sz val="14.0"/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
     </font>
     <font>
-      <sz val="11.0"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-    </font>
-    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
@@ -227,7 +239,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="8">
@@ -311,58 +323,41 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+  <cellXfs count="11">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="2" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="4" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="5" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="6" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="7" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0"/>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
@@ -373,19 +368,17 @@
     <xdr:ext cx="6115050" cy="1400175"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image1.png"/>
+        <xdr:cNvPr id="2" name="image1.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip cstate="print" r:embed="rId1"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
       <xdr:spPr>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
+        <a:prstGeom prst="rect"/>
         <a:noFill/>
       </xdr:spPr>
     </xdr:pic>
@@ -394,16 +387,8 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -485,6 +470,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
+          <a:tileRect/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -511,24 +497,25 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="6350" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="12700" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="19050" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -589,6 +576,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
@@ -597,33 +585,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" topLeftCell="A4"/>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="12.63" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="0.88"/>
-    <col customWidth="1" min="2" max="2" width="25.38"/>
-    <col customWidth="1" min="3" max="3" width="21.38"/>
-    <col customWidth="1" min="4" max="4" width="22.13"/>
-    <col customWidth="1" min="5" max="5" width="26.38"/>
-    <col customWidth="1" min="6" max="6" width="31.88"/>
-    <col customWidth="1" min="7" max="26" width="10.63"/>
+    <col min="1" max="1" width="0.88" customWidth="1"/>
+    <col min="2" max="2" width="25.38" customWidth="1"/>
+    <col min="3" max="3" width="21.38" customWidth="1"/>
+    <col min="4" max="4" width="22.13" customWidth="1"/>
+    <col min="5" max="5" width="26.38" customWidth="1"/>
+    <col min="6" max="6" width="31.88" customWidth="1"/>
+    <col min="7" max="26" width="10.63" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="4.5" customHeight="1"/>
-    <row r="2" ht="120.0" customHeight="1">
+    <row r="2" ht="120" customHeight="1">
       <c r="B2" s="1"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" ht="30.0" customHeight="1">
+    <row r="3" ht="30" customHeight="1">
       <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
@@ -632,7 +617,7 @@
       <c r="E3" s="4"/>
       <c r="F3" s="5"/>
     </row>
-    <row r="4" ht="30.0" customHeight="1">
+    <row r="4" ht="30" customHeight="1">
       <c r="B4" s="6" t="s">
         <v>1</v>
       </c>
@@ -649,7 +634,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" ht="15.0" customHeight="1">
+    <row r="5" ht="15" customHeight="1">
       <c r="A5" s="9"/>
       <c r="B5" s="10" t="s">
         <v>6</v>
@@ -657,7 +642,7 @@
       <c r="C5" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="11"/>
+      <c r="D5" s="9"/>
       <c r="E5" s="10" t="s">
         <v>8</v>
       </c>
@@ -665,7 +650,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" ht="15.0" customHeight="1">
+    <row r="6" ht="15" customHeight="1">
       <c r="A6" s="9"/>
       <c r="B6" s="10" t="s">
         <v>6</v>
@@ -673,13 +658,13 @@
       <c r="C6" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="11"/>
+      <c r="D6" s="9"/>
       <c r="E6" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="11"/>
+      <c r="F6" s="9"/>
     </row>
-    <row r="7" ht="15.0" customHeight="1">
+    <row r="7" ht="15" customHeight="1">
       <c r="A7" s="9"/>
       <c r="B7" s="10" t="s">
         <v>8</v>
@@ -687,7 +672,7 @@
       <c r="C7" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="10" t="s">
         <v>11</v>
       </c>
       <c r="E7" s="10" t="s">
@@ -697,7 +682,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" ht="15.0" customHeight="1">
+    <row r="8" ht="15" customHeight="1">
       <c r="A8" s="9"/>
       <c r="B8" s="10" t="s">
         <v>8</v>
@@ -705,7 +690,7 @@
       <c r="C8" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="10" t="s">
         <v>13</v>
       </c>
       <c r="E8" s="10" t="s">
@@ -715,7 +700,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" ht="15.0" customHeight="1">
+    <row r="9" ht="15" customHeight="1">
       <c r="A9" s="9"/>
       <c r="B9" s="10" t="s">
         <v>8</v>
@@ -729,7 +714,7 @@
       </c>
       <c r="F9" s="9"/>
     </row>
-    <row r="10" ht="15.0" customHeight="1">
+    <row r="10" ht="15" customHeight="1">
       <c r="A10" s="9"/>
       <c r="B10" s="10" t="s">
         <v>14</v>
@@ -745,7 +730,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="11" ht="15.0" customHeight="1">
+    <row r="11" ht="15" customHeight="1">
       <c r="A11" s="9"/>
       <c r="B11" s="10" t="s">
         <v>14</v>
@@ -753,13 +738,13 @@
       <c r="C11" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="11"/>
+      <c r="D11" s="9"/>
       <c r="E11" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="F11" s="11"/>
+      <c r="F11" s="9"/>
     </row>
-    <row r="12" ht="15.0" customHeight="1">
+    <row r="12" ht="15" customHeight="1">
       <c r="A12" s="9"/>
       <c r="B12" s="10" t="s">
         <v>16</v>
@@ -767,7 +752,7 @@
       <c r="C12" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D12" s="10" t="s">
         <v>18</v>
       </c>
       <c r="E12" s="10" t="s">
@@ -777,7 +762,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" ht="15.0" customHeight="1">
+    <row r="13" ht="15" customHeight="1">
       <c r="A13" s="9"/>
       <c r="B13" s="10" t="s">
         <v>16</v>
@@ -785,7 +770,7 @@
       <c r="C13" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D13" s="10" t="s">
         <v>19</v>
       </c>
       <c r="E13" s="10" t="s">
@@ -795,7 +780,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" ht="15.0" customHeight="1">
+    <row r="14" ht="15" customHeight="1">
       <c r="A14" s="9"/>
       <c r="B14" s="10" t="s">
         <v>16</v>
@@ -809,10 +794,6 @@
       </c>
       <c r="F14" s="9"/>
     </row>
-    <row r="15" ht="15.0" customHeight="1"/>
-    <row r="16" ht="15.0" customHeight="1"/>
-    <row r="17" ht="15.0" customHeight="1"/>
-    <row r="18" ht="15.0" customHeight="1"/>
     <row r="19" ht="14.25" customHeight="1"/>
     <row r="20" ht="14.25" customHeight="1"/>
     <row r="21" ht="14.25" customHeight="1"/>
@@ -1802,41 +1783,39 @@
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B3:F3"/>
   </mergeCells>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A7">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="12.63" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="0.88"/>
-    <col customWidth="1" min="2" max="2" width="29.75"/>
-    <col customWidth="1" min="3" max="3" width="27.5"/>
-    <col customWidth="1" min="4" max="4" width="20.75"/>
-    <col customWidth="1" min="5" max="5" width="34.13"/>
-    <col customWidth="1" min="6" max="6" width="53.5"/>
-    <col customWidth="1" min="7" max="26" width="10.63"/>
+    <col min="1" max="1" width="0.88" customWidth="1"/>
+    <col min="2" max="2" width="29.75" customWidth="1"/>
+    <col min="3" max="3" width="27.5" customWidth="1"/>
+    <col min="4" max="4" width="20.75" customWidth="1"/>
+    <col min="5" max="5" width="34.13" customWidth="1"/>
+    <col min="6" max="6" width="53.5" customWidth="1"/>
+    <col min="7" max="26" width="10.63" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="4.5" customHeight="1"/>
-    <row r="2" ht="120.0" customHeight="1">
+    <row r="2" ht="120" customHeight="1">
       <c r="B2" s="1"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
     </row>
-    <row r="3" ht="30.0" customHeight="1">
+    <row r="3" ht="30" customHeight="1">
       <c r="B3" s="3" t="s">
         <v>21</v>
       </c>
@@ -1845,7 +1824,7 @@
       <c r="E3" s="4"/>
       <c r="F3" s="5"/>
     </row>
-    <row r="4" ht="30.0" customHeight="1">
+    <row r="4" ht="30" customHeight="1">
       <c r="B4" s="6" t="s">
         <v>1</v>
       </c>
@@ -1863,117 +1842,1264 @@
       </c>
     </row>
     <row r="5" ht="28.5" customHeight="1">
-      <c r="B5" s="13" t="s">
+      <c r="B5" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="10" t="s">
         <v>23</v>
       </c>
       <c r="D5" s="9"/>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="10" t="s">
         <v>24</v>
       </c>
       <c r="F5" s="9"/>
     </row>
     <row r="6" ht="28.5" customHeight="1">
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="10" t="s">
         <v>25</v>
       </c>
       <c r="D6" s="9"/>
-      <c r="E6" s="13" t="s">
+      <c r="E6" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="F6" s="13" t="s">
+      <c r="F6" s="10" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="7" ht="29.25" customHeight="1">
-      <c r="B7" s="13" t="s">
+    <row r="7" ht="28.5" customHeight="1">
+      <c r="B7" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="9"/>
+      <c r="E7" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="8" ht="29.25" customHeight="1">
+      <c r="B8" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7" s="13" t="s">
+      <c r="C8" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="F8" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" ht="31.5" customHeight="1">
+      <c r="B9" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="10" t="s">
         <v>30</v>
       </c>
+      <c r="D9" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>35</v>
+      </c>
     </row>
-    <row r="8" ht="31.5" customHeight="1">
-      <c r="B8" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="F8" s="13" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" ht="30.0" customHeight="1">
-      <c r="B9" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="C9" s="13" t="s">
+    <row r="10" ht="30" customHeight="1">
+      <c r="B10" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="D9" s="9"/>
-      <c r="E9" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="F9" s="9"/>
-    </row>
-    <row r="10" ht="27.75" customHeight="1">
-      <c r="B10" s="13" t="s">
-        <v>35</v>
-      </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="10" t="s">
         <v>36</v>
       </c>
       <c r="D10" s="9"/>
-      <c r="E10" s="13" t="s">
+      <c r="E10" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="F10" s="13" t="s">
-        <v>38</v>
-      </c>
+      <c r="F10" s="9"/>
     </row>
     <row r="11" ht="27.75" customHeight="1">
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="C11" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="E11" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="F11" s="13" t="s">
+      <c r="C11" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="9"/>
+      <c r="E11" s="10" t="s">
         <v>39</v>
       </c>
+      <c r="F11" s="10" t="s">
+        <v>40</v>
+      </c>
     </row>
-    <row r="12" ht="15.0" customHeight="1"/>
-    <row r="13" ht="15.0" customHeight="1"/>
-    <row r="14" ht="15.0" customHeight="1"/>
-    <row r="15" ht="15.0" customHeight="1"/>
-    <row r="16" ht="15.0" customHeight="1"/>
+    <row r="12" ht="27.75" customHeight="1">
+      <c r="B12" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" ht="30.75" customHeight="1">
+      <c r="B13" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" ht="15" customHeight="1">
+      <c r="B15"/>
+    </row>
+    <row r="18" ht="14.25" customHeight="1"/>
+    <row r="19" ht="14.25" customHeight="1"/>
+    <row r="20" ht="14.25" customHeight="1"/>
+    <row r="21" ht="14.25" customHeight="1"/>
+    <row r="22" ht="14.25" customHeight="1"/>
+    <row r="23" ht="14.25" customHeight="1"/>
+    <row r="24" ht="14.25" customHeight="1"/>
+    <row r="25" ht="14.25" customHeight="1"/>
+    <row r="26" ht="14.25" customHeight="1"/>
+    <row r="27" ht="14.25" customHeight="1"/>
+    <row r="28" ht="14.25" customHeight="1"/>
+    <row r="29" ht="14.25" customHeight="1"/>
+    <row r="30" ht="14.25" customHeight="1"/>
+    <row r="31" ht="14.25" customHeight="1"/>
+    <row r="32" ht="14.25" customHeight="1"/>
+    <row r="33" ht="14.25" customHeight="1"/>
+    <row r="34" ht="14.25" customHeight="1"/>
+    <row r="35" ht="14.25" customHeight="1"/>
+    <row r="36" ht="14.25" customHeight="1"/>
+    <row r="37" ht="14.25" customHeight="1"/>
+    <row r="38" ht="14.25" customHeight="1"/>
+    <row r="39" ht="14.25" customHeight="1"/>
+    <row r="40" ht="14.25" customHeight="1"/>
+    <row r="41" ht="14.25" customHeight="1"/>
+    <row r="42" ht="14.25" customHeight="1"/>
+    <row r="43" ht="14.25" customHeight="1"/>
+    <row r="44" ht="14.25" customHeight="1"/>
+    <row r="45" ht="14.25" customHeight="1"/>
+    <row r="46" ht="14.25" customHeight="1"/>
+    <row r="47" ht="14.25" customHeight="1"/>
+    <row r="48" ht="14.25" customHeight="1"/>
+    <row r="49" ht="14.25" customHeight="1"/>
+    <row r="50" ht="14.25" customHeight="1"/>
+    <row r="51" ht="14.25" customHeight="1"/>
+    <row r="52" ht="14.25" customHeight="1"/>
+    <row r="53" ht="14.25" customHeight="1"/>
+    <row r="54" ht="14.25" customHeight="1"/>
+    <row r="55" ht="14.25" customHeight="1"/>
+    <row r="56" ht="14.25" customHeight="1"/>
+    <row r="57" ht="14.25" customHeight="1"/>
+    <row r="58" ht="14.25" customHeight="1"/>
+    <row r="59" ht="14.25" customHeight="1"/>
+    <row r="60" ht="14.25" customHeight="1"/>
+    <row r="61" ht="14.25" customHeight="1"/>
+    <row r="62" ht="14.25" customHeight="1"/>
+    <row r="63" ht="14.25" customHeight="1"/>
+    <row r="64" ht="14.25" customHeight="1"/>
+    <row r="65" ht="14.25" customHeight="1"/>
+    <row r="66" ht="14.25" customHeight="1"/>
+    <row r="67" ht="14.25" customHeight="1"/>
+    <row r="68" ht="14.25" customHeight="1"/>
+    <row r="69" ht="14.25" customHeight="1"/>
+    <row r="70" ht="14.25" customHeight="1"/>
+    <row r="71" ht="14.25" customHeight="1"/>
+    <row r="72" ht="14.25" customHeight="1"/>
+    <row r="73" ht="14.25" customHeight="1"/>
+    <row r="74" ht="14.25" customHeight="1"/>
+    <row r="75" ht="14.25" customHeight="1"/>
+    <row r="76" ht="14.25" customHeight="1"/>
+    <row r="77" ht="14.25" customHeight="1"/>
+    <row r="78" ht="14.25" customHeight="1"/>
+    <row r="79" ht="14.25" customHeight="1"/>
+    <row r="80" ht="14.25" customHeight="1"/>
+    <row r="81" ht="14.25" customHeight="1"/>
+    <row r="82" ht="14.25" customHeight="1"/>
+    <row r="83" ht="14.25" customHeight="1"/>
+    <row r="84" ht="14.25" customHeight="1"/>
+    <row r="85" ht="14.25" customHeight="1"/>
+    <row r="86" ht="14.25" customHeight="1"/>
+    <row r="87" ht="14.25" customHeight="1"/>
+    <row r="88" ht="14.25" customHeight="1"/>
+    <row r="89" ht="14.25" customHeight="1"/>
+    <row r="90" ht="14.25" customHeight="1"/>
+    <row r="91" ht="14.25" customHeight="1"/>
+    <row r="92" ht="14.25" customHeight="1"/>
+    <row r="93" ht="14.25" customHeight="1"/>
+    <row r="94" ht="14.25" customHeight="1"/>
+    <row r="95" ht="14.25" customHeight="1"/>
+    <row r="96" ht="14.25" customHeight="1"/>
+    <row r="97" ht="14.25" customHeight="1"/>
+    <row r="98" ht="14.25" customHeight="1"/>
+    <row r="99" ht="14.25" customHeight="1"/>
+    <row r="100" ht="14.25" customHeight="1"/>
+    <row r="101" ht="14.25" customHeight="1"/>
+    <row r="102" ht="14.25" customHeight="1"/>
+    <row r="103" ht="14.25" customHeight="1"/>
+    <row r="104" ht="14.25" customHeight="1"/>
+    <row r="105" ht="14.25" customHeight="1"/>
+    <row r="106" ht="14.25" customHeight="1"/>
+    <row r="107" ht="14.25" customHeight="1"/>
+    <row r="108" ht="14.25" customHeight="1"/>
+    <row r="109" ht="14.25" customHeight="1"/>
+    <row r="110" ht="14.25" customHeight="1"/>
+    <row r="111" ht="14.25" customHeight="1"/>
+    <row r="112" ht="14.25" customHeight="1"/>
+    <row r="113" ht="14.25" customHeight="1"/>
+    <row r="114" ht="14.25" customHeight="1"/>
+    <row r="115" ht="14.25" customHeight="1"/>
+    <row r="116" ht="14.25" customHeight="1"/>
+    <row r="117" ht="14.25" customHeight="1"/>
+    <row r="118" ht="14.25" customHeight="1"/>
+    <row r="119" ht="14.25" customHeight="1"/>
+    <row r="120" ht="14.25" customHeight="1"/>
+    <row r="121" ht="14.25" customHeight="1"/>
+    <row r="122" ht="14.25" customHeight="1"/>
+    <row r="123" ht="14.25" customHeight="1"/>
+    <row r="124" ht="14.25" customHeight="1"/>
+    <row r="125" ht="14.25" customHeight="1"/>
+    <row r="126" ht="14.25" customHeight="1"/>
+    <row r="127" ht="14.25" customHeight="1"/>
+    <row r="128" ht="14.25" customHeight="1"/>
+    <row r="129" ht="14.25" customHeight="1"/>
+    <row r="130" ht="14.25" customHeight="1"/>
+    <row r="131" ht="14.25" customHeight="1"/>
+    <row r="132" ht="14.25" customHeight="1"/>
+    <row r="133" ht="14.25" customHeight="1"/>
+    <row r="134" ht="14.25" customHeight="1"/>
+    <row r="135" ht="14.25" customHeight="1"/>
+    <row r="136" ht="14.25" customHeight="1"/>
+    <row r="137" ht="14.25" customHeight="1"/>
+    <row r="138" ht="14.25" customHeight="1"/>
+    <row r="139" ht="14.25" customHeight="1"/>
+    <row r="140" ht="14.25" customHeight="1"/>
+    <row r="141" ht="14.25" customHeight="1"/>
+    <row r="142" ht="14.25" customHeight="1"/>
+    <row r="143" ht="14.25" customHeight="1"/>
+    <row r="144" ht="14.25" customHeight="1"/>
+    <row r="145" ht="14.25" customHeight="1"/>
+    <row r="146" ht="14.25" customHeight="1"/>
+    <row r="147" ht="14.25" customHeight="1"/>
+    <row r="148" ht="14.25" customHeight="1"/>
+    <row r="149" ht="14.25" customHeight="1"/>
+    <row r="150" ht="14.25" customHeight="1"/>
+    <row r="151" ht="14.25" customHeight="1"/>
+    <row r="152" ht="14.25" customHeight="1"/>
+    <row r="153" ht="14.25" customHeight="1"/>
+    <row r="154" ht="14.25" customHeight="1"/>
+    <row r="155" ht="14.25" customHeight="1"/>
+    <row r="156" ht="14.25" customHeight="1"/>
+    <row r="157" ht="14.25" customHeight="1"/>
+    <row r="158" ht="14.25" customHeight="1"/>
+    <row r="159" ht="14.25" customHeight="1"/>
+    <row r="160" ht="14.25" customHeight="1"/>
+    <row r="161" ht="14.25" customHeight="1"/>
+    <row r="162" ht="14.25" customHeight="1"/>
+    <row r="163" ht="14.25" customHeight="1"/>
+    <row r="164" ht="14.25" customHeight="1"/>
+    <row r="165" ht="14.25" customHeight="1"/>
+    <row r="166" ht="14.25" customHeight="1"/>
+    <row r="167" ht="14.25" customHeight="1"/>
+    <row r="168" ht="14.25" customHeight="1"/>
+    <row r="169" ht="14.25" customHeight="1"/>
+    <row r="170" ht="14.25" customHeight="1"/>
+    <row r="171" ht="14.25" customHeight="1"/>
+    <row r="172" ht="14.25" customHeight="1"/>
+    <row r="173" ht="14.25" customHeight="1"/>
+    <row r="174" ht="14.25" customHeight="1"/>
+    <row r="175" ht="14.25" customHeight="1"/>
+    <row r="176" ht="14.25" customHeight="1"/>
+    <row r="177" ht="14.25" customHeight="1"/>
+    <row r="178" ht="14.25" customHeight="1"/>
+    <row r="179" ht="14.25" customHeight="1"/>
+    <row r="180" ht="14.25" customHeight="1"/>
+    <row r="181" ht="14.25" customHeight="1"/>
+    <row r="182" ht="14.25" customHeight="1"/>
+    <row r="183" ht="14.25" customHeight="1"/>
+    <row r="184" ht="14.25" customHeight="1"/>
+    <row r="185" ht="14.25" customHeight="1"/>
+    <row r="186" ht="14.25" customHeight="1"/>
+    <row r="187" ht="14.25" customHeight="1"/>
+    <row r="188" ht="14.25" customHeight="1"/>
+    <row r="189" ht="14.25" customHeight="1"/>
+    <row r="190" ht="14.25" customHeight="1"/>
+    <row r="191" ht="14.25" customHeight="1"/>
+    <row r="192" ht="14.25" customHeight="1"/>
+    <row r="193" ht="14.25" customHeight="1"/>
+    <row r="194" ht="14.25" customHeight="1"/>
+    <row r="195" ht="14.25" customHeight="1"/>
+    <row r="196" ht="14.25" customHeight="1"/>
+    <row r="197" ht="14.25" customHeight="1"/>
+    <row r="198" ht="14.25" customHeight="1"/>
+    <row r="199" ht="14.25" customHeight="1"/>
+    <row r="200" ht="14.25" customHeight="1"/>
+    <row r="201" ht="14.25" customHeight="1"/>
+    <row r="202" ht="14.25" customHeight="1"/>
+    <row r="203" ht="14.25" customHeight="1"/>
+    <row r="204" ht="14.25" customHeight="1"/>
+    <row r="205" ht="14.25" customHeight="1"/>
+    <row r="206" ht="14.25" customHeight="1"/>
+    <row r="207" ht="14.25" customHeight="1"/>
+    <row r="208" ht="14.25" customHeight="1"/>
+    <row r="209" ht="14.25" customHeight="1"/>
+    <row r="210" ht="14.25" customHeight="1"/>
+    <row r="211" ht="14.25" customHeight="1"/>
+    <row r="212" ht="14.25" customHeight="1"/>
+    <row r="213" ht="14.25" customHeight="1"/>
+    <row r="214" ht="14.25" customHeight="1"/>
+    <row r="215" ht="14.25" customHeight="1"/>
+    <row r="216" ht="14.25" customHeight="1"/>
+    <row r="217" ht="14.25" customHeight="1"/>
+    <row r="218" ht="14.25" customHeight="1"/>
+    <row r="219" ht="14.25" customHeight="1"/>
+    <row r="220" ht="14.25" customHeight="1"/>
+    <row r="221" ht="14.25" customHeight="1"/>
+    <row r="222" ht="14.25" customHeight="1"/>
+    <row r="223" ht="14.25" customHeight="1"/>
+    <row r="224" ht="14.25" customHeight="1"/>
+    <row r="225" ht="14.25" customHeight="1"/>
+    <row r="226" ht="14.25" customHeight="1"/>
+    <row r="227" ht="14.25" customHeight="1"/>
+    <row r="228" ht="14.25" customHeight="1"/>
+    <row r="229" ht="14.25" customHeight="1"/>
+    <row r="230" ht="14.25" customHeight="1"/>
+    <row r="231" ht="14.25" customHeight="1"/>
+    <row r="232" ht="14.25" customHeight="1"/>
+    <row r="233" ht="14.25" customHeight="1"/>
+    <row r="234" ht="14.25" customHeight="1"/>
+    <row r="235" ht="14.25" customHeight="1"/>
+    <row r="236" ht="14.25" customHeight="1"/>
+    <row r="237" ht="14.25" customHeight="1"/>
+    <row r="238" ht="14.25" customHeight="1"/>
+    <row r="239" ht="14.25" customHeight="1"/>
+    <row r="240" ht="14.25" customHeight="1"/>
+    <row r="241" ht="14.25" customHeight="1"/>
+    <row r="242" ht="14.25" customHeight="1"/>
+    <row r="243" ht="14.25" customHeight="1"/>
+    <row r="244" ht="14.25" customHeight="1"/>
+    <row r="245" ht="14.25" customHeight="1"/>
+    <row r="246" ht="14.25" customHeight="1"/>
+    <row r="247" ht="14.25" customHeight="1"/>
+    <row r="248" ht="14.25" customHeight="1"/>
+    <row r="249" ht="14.25" customHeight="1"/>
+    <row r="250" ht="14.25" customHeight="1"/>
+    <row r="251" ht="14.25" customHeight="1"/>
+    <row r="252" ht="14.25" customHeight="1"/>
+    <row r="253" ht="14.25" customHeight="1"/>
+    <row r="254" ht="14.25" customHeight="1"/>
+    <row r="255" ht="14.25" customHeight="1"/>
+    <row r="256" ht="14.25" customHeight="1"/>
+    <row r="257" ht="14.25" customHeight="1"/>
+    <row r="258" ht="14.25" customHeight="1"/>
+    <row r="259" ht="14.25" customHeight="1"/>
+    <row r="260" ht="14.25" customHeight="1"/>
+    <row r="261" ht="14.25" customHeight="1"/>
+    <row r="262" ht="14.25" customHeight="1"/>
+    <row r="263" ht="14.25" customHeight="1"/>
+    <row r="264" ht="14.25" customHeight="1"/>
+    <row r="265" ht="14.25" customHeight="1"/>
+    <row r="266" ht="14.25" customHeight="1"/>
+    <row r="267" ht="14.25" customHeight="1"/>
+    <row r="268" ht="14.25" customHeight="1"/>
+    <row r="269" ht="14.25" customHeight="1"/>
+    <row r="270" ht="14.25" customHeight="1"/>
+    <row r="271" ht="14.25" customHeight="1"/>
+    <row r="272" ht="14.25" customHeight="1"/>
+    <row r="273" ht="14.25" customHeight="1"/>
+    <row r="274" ht="14.25" customHeight="1"/>
+    <row r="275" ht="14.25" customHeight="1"/>
+    <row r="276" ht="14.25" customHeight="1"/>
+    <row r="277" ht="14.25" customHeight="1"/>
+    <row r="278" ht="14.25" customHeight="1"/>
+    <row r="279" ht="14.25" customHeight="1"/>
+    <row r="280" ht="14.25" customHeight="1"/>
+    <row r="281" ht="14.25" customHeight="1"/>
+    <row r="282" ht="14.25" customHeight="1"/>
+    <row r="283" ht="14.25" customHeight="1"/>
+    <row r="284" ht="14.25" customHeight="1"/>
+    <row r="285" ht="14.25" customHeight="1"/>
+    <row r="286" ht="14.25" customHeight="1"/>
+    <row r="287" ht="14.25" customHeight="1"/>
+    <row r="288" ht="14.25" customHeight="1"/>
+    <row r="289" ht="14.25" customHeight="1"/>
+    <row r="290" ht="14.25" customHeight="1"/>
+    <row r="291" ht="14.25" customHeight="1"/>
+    <row r="292" ht="14.25" customHeight="1"/>
+    <row r="293" ht="14.25" customHeight="1"/>
+    <row r="294" ht="14.25" customHeight="1"/>
+    <row r="295" ht="14.25" customHeight="1"/>
+    <row r="296" ht="14.25" customHeight="1"/>
+    <row r="297" ht="14.25" customHeight="1"/>
+    <row r="298" ht="14.25" customHeight="1"/>
+    <row r="299" ht="14.25" customHeight="1"/>
+    <row r="300" ht="14.25" customHeight="1"/>
+    <row r="301" ht="14.25" customHeight="1"/>
+    <row r="302" ht="14.25" customHeight="1"/>
+    <row r="303" ht="14.25" customHeight="1"/>
+    <row r="304" ht="14.25" customHeight="1"/>
+    <row r="305" ht="14.25" customHeight="1"/>
+    <row r="306" ht="14.25" customHeight="1"/>
+    <row r="307" ht="14.25" customHeight="1"/>
+    <row r="308" ht="14.25" customHeight="1"/>
+    <row r="309" ht="14.25" customHeight="1"/>
+    <row r="310" ht="14.25" customHeight="1"/>
+    <row r="311" ht="14.25" customHeight="1"/>
+    <row r="312" ht="14.25" customHeight="1"/>
+    <row r="313" ht="14.25" customHeight="1"/>
+    <row r="314" ht="14.25" customHeight="1"/>
+    <row r="315" ht="14.25" customHeight="1"/>
+    <row r="316" ht="14.25" customHeight="1"/>
+    <row r="317" ht="14.25" customHeight="1"/>
+    <row r="318" ht="14.25" customHeight="1"/>
+    <row r="319" ht="14.25" customHeight="1"/>
+    <row r="320" ht="14.25" customHeight="1"/>
+    <row r="321" ht="14.25" customHeight="1"/>
+    <row r="322" ht="14.25" customHeight="1"/>
+    <row r="323" ht="14.25" customHeight="1"/>
+    <row r="324" ht="14.25" customHeight="1"/>
+    <row r="325" ht="14.25" customHeight="1"/>
+    <row r="326" ht="14.25" customHeight="1"/>
+    <row r="327" ht="14.25" customHeight="1"/>
+    <row r="328" ht="14.25" customHeight="1"/>
+    <row r="329" ht="14.25" customHeight="1"/>
+    <row r="330" ht="14.25" customHeight="1"/>
+    <row r="331" ht="14.25" customHeight="1"/>
+    <row r="332" ht="14.25" customHeight="1"/>
+    <row r="333" ht="14.25" customHeight="1"/>
+    <row r="334" ht="14.25" customHeight="1"/>
+    <row r="335" ht="14.25" customHeight="1"/>
+    <row r="336" ht="14.25" customHeight="1"/>
+    <row r="337" ht="14.25" customHeight="1"/>
+    <row r="338" ht="14.25" customHeight="1"/>
+    <row r="339" ht="14.25" customHeight="1"/>
+    <row r="340" ht="14.25" customHeight="1"/>
+    <row r="341" ht="14.25" customHeight="1"/>
+    <row r="342" ht="14.25" customHeight="1"/>
+    <row r="343" ht="14.25" customHeight="1"/>
+    <row r="344" ht="14.25" customHeight="1"/>
+    <row r="345" ht="14.25" customHeight="1"/>
+    <row r="346" ht="14.25" customHeight="1"/>
+    <row r="347" ht="14.25" customHeight="1"/>
+    <row r="348" ht="14.25" customHeight="1"/>
+    <row r="349" ht="14.25" customHeight="1"/>
+    <row r="350" ht="14.25" customHeight="1"/>
+    <row r="351" ht="14.25" customHeight="1"/>
+    <row r="352" ht="14.25" customHeight="1"/>
+    <row r="353" ht="14.25" customHeight="1"/>
+    <row r="354" ht="14.25" customHeight="1"/>
+    <row r="355" ht="14.25" customHeight="1"/>
+    <row r="356" ht="14.25" customHeight="1"/>
+    <row r="357" ht="14.25" customHeight="1"/>
+    <row r="358" ht="14.25" customHeight="1"/>
+    <row r="359" ht="14.25" customHeight="1"/>
+    <row r="360" ht="14.25" customHeight="1"/>
+    <row r="361" ht="14.25" customHeight="1"/>
+    <row r="362" ht="14.25" customHeight="1"/>
+    <row r="363" ht="14.25" customHeight="1"/>
+    <row r="364" ht="14.25" customHeight="1"/>
+    <row r="365" ht="14.25" customHeight="1"/>
+    <row r="366" ht="14.25" customHeight="1"/>
+    <row r="367" ht="14.25" customHeight="1"/>
+    <row r="368" ht="14.25" customHeight="1"/>
+    <row r="369" ht="14.25" customHeight="1"/>
+    <row r="370" ht="14.25" customHeight="1"/>
+    <row r="371" ht="14.25" customHeight="1"/>
+    <row r="372" ht="14.25" customHeight="1"/>
+    <row r="373" ht="14.25" customHeight="1"/>
+    <row r="374" ht="14.25" customHeight="1"/>
+    <row r="375" ht="14.25" customHeight="1"/>
+    <row r="376" ht="14.25" customHeight="1"/>
+    <row r="377" ht="14.25" customHeight="1"/>
+    <row r="378" ht="14.25" customHeight="1"/>
+    <row r="379" ht="14.25" customHeight="1"/>
+    <row r="380" ht="14.25" customHeight="1"/>
+    <row r="381" ht="14.25" customHeight="1"/>
+    <row r="382" ht="14.25" customHeight="1"/>
+    <row r="383" ht="14.25" customHeight="1"/>
+    <row r="384" ht="14.25" customHeight="1"/>
+    <row r="385" ht="14.25" customHeight="1"/>
+    <row r="386" ht="14.25" customHeight="1"/>
+    <row r="387" ht="14.25" customHeight="1"/>
+    <row r="388" ht="14.25" customHeight="1"/>
+    <row r="389" ht="14.25" customHeight="1"/>
+    <row r="390" ht="14.25" customHeight="1"/>
+    <row r="391" ht="14.25" customHeight="1"/>
+    <row r="392" ht="14.25" customHeight="1"/>
+    <row r="393" ht="14.25" customHeight="1"/>
+    <row r="394" ht="14.25" customHeight="1"/>
+    <row r="395" ht="14.25" customHeight="1"/>
+    <row r="396" ht="14.25" customHeight="1"/>
+    <row r="397" ht="14.25" customHeight="1"/>
+    <row r="398" ht="14.25" customHeight="1"/>
+    <row r="399" ht="14.25" customHeight="1"/>
+    <row r="400" ht="14.25" customHeight="1"/>
+    <row r="401" ht="14.25" customHeight="1"/>
+    <row r="402" ht="14.25" customHeight="1"/>
+    <row r="403" ht="14.25" customHeight="1"/>
+    <row r="404" ht="14.25" customHeight="1"/>
+    <row r="405" ht="14.25" customHeight="1"/>
+    <row r="406" ht="14.25" customHeight="1"/>
+    <row r="407" ht="14.25" customHeight="1"/>
+    <row r="408" ht="14.25" customHeight="1"/>
+    <row r="409" ht="14.25" customHeight="1"/>
+    <row r="410" ht="14.25" customHeight="1"/>
+    <row r="411" ht="14.25" customHeight="1"/>
+    <row r="412" ht="14.25" customHeight="1"/>
+    <row r="413" ht="14.25" customHeight="1"/>
+    <row r="414" ht="14.25" customHeight="1"/>
+    <row r="415" ht="14.25" customHeight="1"/>
+    <row r="416" ht="14.25" customHeight="1"/>
+    <row r="417" ht="14.25" customHeight="1"/>
+    <row r="418" ht="14.25" customHeight="1"/>
+    <row r="419" ht="14.25" customHeight="1"/>
+    <row r="420" ht="14.25" customHeight="1"/>
+    <row r="421" ht="14.25" customHeight="1"/>
+    <row r="422" ht="14.25" customHeight="1"/>
+    <row r="423" ht="14.25" customHeight="1"/>
+    <row r="424" ht="14.25" customHeight="1"/>
+    <row r="425" ht="14.25" customHeight="1"/>
+    <row r="426" ht="14.25" customHeight="1"/>
+    <row r="427" ht="14.25" customHeight="1"/>
+    <row r="428" ht="14.25" customHeight="1"/>
+    <row r="429" ht="14.25" customHeight="1"/>
+    <row r="430" ht="14.25" customHeight="1"/>
+    <row r="431" ht="14.25" customHeight="1"/>
+    <row r="432" ht="14.25" customHeight="1"/>
+    <row r="433" ht="14.25" customHeight="1"/>
+    <row r="434" ht="14.25" customHeight="1"/>
+    <row r="435" ht="14.25" customHeight="1"/>
+    <row r="436" ht="14.25" customHeight="1"/>
+    <row r="437" ht="14.25" customHeight="1"/>
+    <row r="438" ht="14.25" customHeight="1"/>
+    <row r="439" ht="14.25" customHeight="1"/>
+    <row r="440" ht="14.25" customHeight="1"/>
+    <row r="441" ht="14.25" customHeight="1"/>
+    <row r="442" ht="14.25" customHeight="1"/>
+    <row r="443" ht="14.25" customHeight="1"/>
+    <row r="444" ht="14.25" customHeight="1"/>
+    <row r="445" ht="14.25" customHeight="1"/>
+    <row r="446" ht="14.25" customHeight="1"/>
+    <row r="447" ht="14.25" customHeight="1"/>
+    <row r="448" ht="14.25" customHeight="1"/>
+    <row r="449" ht="14.25" customHeight="1"/>
+    <row r="450" ht="14.25" customHeight="1"/>
+    <row r="451" ht="14.25" customHeight="1"/>
+    <row r="452" ht="14.25" customHeight="1"/>
+    <row r="453" ht="14.25" customHeight="1"/>
+    <row r="454" ht="14.25" customHeight="1"/>
+    <row r="455" ht="14.25" customHeight="1"/>
+    <row r="456" ht="14.25" customHeight="1"/>
+    <row r="457" ht="14.25" customHeight="1"/>
+    <row r="458" ht="14.25" customHeight="1"/>
+    <row r="459" ht="14.25" customHeight="1"/>
+    <row r="460" ht="14.25" customHeight="1"/>
+    <row r="461" ht="14.25" customHeight="1"/>
+    <row r="462" ht="14.25" customHeight="1"/>
+    <row r="463" ht="14.25" customHeight="1"/>
+    <row r="464" ht="14.25" customHeight="1"/>
+    <row r="465" ht="14.25" customHeight="1"/>
+    <row r="466" ht="14.25" customHeight="1"/>
+    <row r="467" ht="14.25" customHeight="1"/>
+    <row r="468" ht="14.25" customHeight="1"/>
+    <row r="469" ht="14.25" customHeight="1"/>
+    <row r="470" ht="14.25" customHeight="1"/>
+    <row r="471" ht="14.25" customHeight="1"/>
+    <row r="472" ht="14.25" customHeight="1"/>
+    <row r="473" ht="14.25" customHeight="1"/>
+    <row r="474" ht="14.25" customHeight="1"/>
+    <row r="475" ht="14.25" customHeight="1"/>
+    <row r="476" ht="14.25" customHeight="1"/>
+    <row r="477" ht="14.25" customHeight="1"/>
+    <row r="478" ht="14.25" customHeight="1"/>
+    <row r="479" ht="14.25" customHeight="1"/>
+    <row r="480" ht="14.25" customHeight="1"/>
+    <row r="481" ht="14.25" customHeight="1"/>
+    <row r="482" ht="14.25" customHeight="1"/>
+    <row r="483" ht="14.25" customHeight="1"/>
+    <row r="484" ht="14.25" customHeight="1"/>
+    <row r="485" ht="14.25" customHeight="1"/>
+    <row r="486" ht="14.25" customHeight="1"/>
+    <row r="487" ht="14.25" customHeight="1"/>
+    <row r="488" ht="14.25" customHeight="1"/>
+    <row r="489" ht="14.25" customHeight="1"/>
+    <row r="490" ht="14.25" customHeight="1"/>
+    <row r="491" ht="14.25" customHeight="1"/>
+    <row r="492" ht="14.25" customHeight="1"/>
+    <row r="493" ht="14.25" customHeight="1"/>
+    <row r="494" ht="14.25" customHeight="1"/>
+    <row r="495" ht="14.25" customHeight="1"/>
+    <row r="496" ht="14.25" customHeight="1"/>
+    <row r="497" ht="14.25" customHeight="1"/>
+    <row r="498" ht="14.25" customHeight="1"/>
+    <row r="499" ht="14.25" customHeight="1"/>
+    <row r="500" ht="14.25" customHeight="1"/>
+    <row r="501" ht="14.25" customHeight="1"/>
+    <row r="502" ht="14.25" customHeight="1"/>
+    <row r="503" ht="14.25" customHeight="1"/>
+    <row r="504" ht="14.25" customHeight="1"/>
+    <row r="505" ht="14.25" customHeight="1"/>
+    <row r="506" ht="14.25" customHeight="1"/>
+    <row r="507" ht="14.25" customHeight="1"/>
+    <row r="508" ht="14.25" customHeight="1"/>
+    <row r="509" ht="14.25" customHeight="1"/>
+    <row r="510" ht="14.25" customHeight="1"/>
+    <row r="511" ht="14.25" customHeight="1"/>
+    <row r="512" ht="14.25" customHeight="1"/>
+    <row r="513" ht="14.25" customHeight="1"/>
+    <row r="514" ht="14.25" customHeight="1"/>
+    <row r="515" ht="14.25" customHeight="1"/>
+    <row r="516" ht="14.25" customHeight="1"/>
+    <row r="517" ht="14.25" customHeight="1"/>
+    <row r="518" ht="14.25" customHeight="1"/>
+    <row r="519" ht="14.25" customHeight="1"/>
+    <row r="520" ht="14.25" customHeight="1"/>
+    <row r="521" ht="14.25" customHeight="1"/>
+    <row r="522" ht="14.25" customHeight="1"/>
+    <row r="523" ht="14.25" customHeight="1"/>
+    <row r="524" ht="14.25" customHeight="1"/>
+    <row r="525" ht="14.25" customHeight="1"/>
+    <row r="526" ht="14.25" customHeight="1"/>
+    <row r="527" ht="14.25" customHeight="1"/>
+    <row r="528" ht="14.25" customHeight="1"/>
+    <row r="529" ht="14.25" customHeight="1"/>
+    <row r="530" ht="14.25" customHeight="1"/>
+    <row r="531" ht="14.25" customHeight="1"/>
+    <row r="532" ht="14.25" customHeight="1"/>
+    <row r="533" ht="14.25" customHeight="1"/>
+    <row r="534" ht="14.25" customHeight="1"/>
+    <row r="535" ht="14.25" customHeight="1"/>
+    <row r="536" ht="14.25" customHeight="1"/>
+    <row r="537" ht="14.25" customHeight="1"/>
+    <row r="538" ht="14.25" customHeight="1"/>
+    <row r="539" ht="14.25" customHeight="1"/>
+    <row r="540" ht="14.25" customHeight="1"/>
+    <row r="541" ht="14.25" customHeight="1"/>
+    <row r="542" ht="14.25" customHeight="1"/>
+    <row r="543" ht="14.25" customHeight="1"/>
+    <row r="544" ht="14.25" customHeight="1"/>
+    <row r="545" ht="14.25" customHeight="1"/>
+    <row r="546" ht="14.25" customHeight="1"/>
+    <row r="547" ht="14.25" customHeight="1"/>
+    <row r="548" ht="14.25" customHeight="1"/>
+    <row r="549" ht="14.25" customHeight="1"/>
+    <row r="550" ht="14.25" customHeight="1"/>
+    <row r="551" ht="14.25" customHeight="1"/>
+    <row r="552" ht="14.25" customHeight="1"/>
+    <row r="553" ht="14.25" customHeight="1"/>
+    <row r="554" ht="14.25" customHeight="1"/>
+    <row r="555" ht="14.25" customHeight="1"/>
+    <row r="556" ht="14.25" customHeight="1"/>
+    <row r="557" ht="14.25" customHeight="1"/>
+    <row r="558" ht="14.25" customHeight="1"/>
+    <row r="559" ht="14.25" customHeight="1"/>
+    <row r="560" ht="14.25" customHeight="1"/>
+    <row r="561" ht="14.25" customHeight="1"/>
+    <row r="562" ht="14.25" customHeight="1"/>
+    <row r="563" ht="14.25" customHeight="1"/>
+    <row r="564" ht="14.25" customHeight="1"/>
+    <row r="565" ht="14.25" customHeight="1"/>
+    <row r="566" ht="14.25" customHeight="1"/>
+    <row r="567" ht="14.25" customHeight="1"/>
+    <row r="568" ht="14.25" customHeight="1"/>
+    <row r="569" ht="14.25" customHeight="1"/>
+    <row r="570" ht="14.25" customHeight="1"/>
+    <row r="571" ht="14.25" customHeight="1"/>
+    <row r="572" ht="14.25" customHeight="1"/>
+    <row r="573" ht="14.25" customHeight="1"/>
+    <row r="574" ht="14.25" customHeight="1"/>
+    <row r="575" ht="14.25" customHeight="1"/>
+    <row r="576" ht="14.25" customHeight="1"/>
+    <row r="577" ht="14.25" customHeight="1"/>
+    <row r="578" ht="14.25" customHeight="1"/>
+    <row r="579" ht="14.25" customHeight="1"/>
+    <row r="580" ht="14.25" customHeight="1"/>
+    <row r="581" ht="14.25" customHeight="1"/>
+    <row r="582" ht="14.25" customHeight="1"/>
+    <row r="583" ht="14.25" customHeight="1"/>
+    <row r="584" ht="14.25" customHeight="1"/>
+    <row r="585" ht="14.25" customHeight="1"/>
+    <row r="586" ht="14.25" customHeight="1"/>
+    <row r="587" ht="14.25" customHeight="1"/>
+    <row r="588" ht="14.25" customHeight="1"/>
+    <row r="589" ht="14.25" customHeight="1"/>
+    <row r="590" ht="14.25" customHeight="1"/>
+    <row r="591" ht="14.25" customHeight="1"/>
+    <row r="592" ht="14.25" customHeight="1"/>
+    <row r="593" ht="14.25" customHeight="1"/>
+    <row r="594" ht="14.25" customHeight="1"/>
+    <row r="595" ht="14.25" customHeight="1"/>
+    <row r="596" ht="14.25" customHeight="1"/>
+    <row r="597" ht="14.25" customHeight="1"/>
+    <row r="598" ht="14.25" customHeight="1"/>
+    <row r="599" ht="14.25" customHeight="1"/>
+    <row r="600" ht="14.25" customHeight="1"/>
+    <row r="601" ht="14.25" customHeight="1"/>
+    <row r="602" ht="14.25" customHeight="1"/>
+    <row r="603" ht="14.25" customHeight="1"/>
+    <row r="604" ht="14.25" customHeight="1"/>
+    <row r="605" ht="14.25" customHeight="1"/>
+    <row r="606" ht="14.25" customHeight="1"/>
+    <row r="607" ht="14.25" customHeight="1"/>
+    <row r="608" ht="14.25" customHeight="1"/>
+    <row r="609" ht="14.25" customHeight="1"/>
+    <row r="610" ht="14.25" customHeight="1"/>
+    <row r="611" ht="14.25" customHeight="1"/>
+    <row r="612" ht="14.25" customHeight="1"/>
+    <row r="613" ht="14.25" customHeight="1"/>
+    <row r="614" ht="14.25" customHeight="1"/>
+    <row r="615" ht="14.25" customHeight="1"/>
+    <row r="616" ht="14.25" customHeight="1"/>
+    <row r="617" ht="14.25" customHeight="1"/>
+    <row r="618" ht="14.25" customHeight="1"/>
+    <row r="619" ht="14.25" customHeight="1"/>
+    <row r="620" ht="14.25" customHeight="1"/>
+    <row r="621" ht="14.25" customHeight="1"/>
+    <row r="622" ht="14.25" customHeight="1"/>
+    <row r="623" ht="14.25" customHeight="1"/>
+    <row r="624" ht="14.25" customHeight="1"/>
+    <row r="625" ht="14.25" customHeight="1"/>
+    <row r="626" ht="14.25" customHeight="1"/>
+    <row r="627" ht="14.25" customHeight="1"/>
+    <row r="628" ht="14.25" customHeight="1"/>
+    <row r="629" ht="14.25" customHeight="1"/>
+    <row r="630" ht="14.25" customHeight="1"/>
+    <row r="631" ht="14.25" customHeight="1"/>
+    <row r="632" ht="14.25" customHeight="1"/>
+    <row r="633" ht="14.25" customHeight="1"/>
+    <row r="634" ht="14.25" customHeight="1"/>
+    <row r="635" ht="14.25" customHeight="1"/>
+    <row r="636" ht="14.25" customHeight="1"/>
+    <row r="637" ht="14.25" customHeight="1"/>
+    <row r="638" ht="14.25" customHeight="1"/>
+    <row r="639" ht="14.25" customHeight="1"/>
+    <row r="640" ht="14.25" customHeight="1"/>
+    <row r="641" ht="14.25" customHeight="1"/>
+    <row r="642" ht="14.25" customHeight="1"/>
+    <row r="643" ht="14.25" customHeight="1"/>
+    <row r="644" ht="14.25" customHeight="1"/>
+    <row r="645" ht="14.25" customHeight="1"/>
+    <row r="646" ht="14.25" customHeight="1"/>
+    <row r="647" ht="14.25" customHeight="1"/>
+    <row r="648" ht="14.25" customHeight="1"/>
+    <row r="649" ht="14.25" customHeight="1"/>
+    <row r="650" ht="14.25" customHeight="1"/>
+    <row r="651" ht="14.25" customHeight="1"/>
+    <row r="652" ht="14.25" customHeight="1"/>
+    <row r="653" ht="14.25" customHeight="1"/>
+    <row r="654" ht="14.25" customHeight="1"/>
+    <row r="655" ht="14.25" customHeight="1"/>
+    <row r="656" ht="14.25" customHeight="1"/>
+    <row r="657" ht="14.25" customHeight="1"/>
+    <row r="658" ht="14.25" customHeight="1"/>
+    <row r="659" ht="14.25" customHeight="1"/>
+    <row r="660" ht="14.25" customHeight="1"/>
+    <row r="661" ht="14.25" customHeight="1"/>
+    <row r="662" ht="14.25" customHeight="1"/>
+    <row r="663" ht="14.25" customHeight="1"/>
+    <row r="664" ht="14.25" customHeight="1"/>
+    <row r="665" ht="14.25" customHeight="1"/>
+    <row r="666" ht="14.25" customHeight="1"/>
+    <row r="667" ht="14.25" customHeight="1"/>
+    <row r="668" ht="14.25" customHeight="1"/>
+    <row r="669" ht="14.25" customHeight="1"/>
+    <row r="670" ht="14.25" customHeight="1"/>
+    <row r="671" ht="14.25" customHeight="1"/>
+    <row r="672" ht="14.25" customHeight="1"/>
+    <row r="673" ht="14.25" customHeight="1"/>
+    <row r="674" ht="14.25" customHeight="1"/>
+    <row r="675" ht="14.25" customHeight="1"/>
+    <row r="676" ht="14.25" customHeight="1"/>
+    <row r="677" ht="14.25" customHeight="1"/>
+    <row r="678" ht="14.25" customHeight="1"/>
+    <row r="679" ht="14.25" customHeight="1"/>
+    <row r="680" ht="14.25" customHeight="1"/>
+    <row r="681" ht="14.25" customHeight="1"/>
+    <row r="682" ht="14.25" customHeight="1"/>
+    <row r="683" ht="14.25" customHeight="1"/>
+    <row r="684" ht="14.25" customHeight="1"/>
+    <row r="685" ht="14.25" customHeight="1"/>
+    <row r="686" ht="14.25" customHeight="1"/>
+    <row r="687" ht="14.25" customHeight="1"/>
+    <row r="688" ht="14.25" customHeight="1"/>
+    <row r="689" ht="14.25" customHeight="1"/>
+    <row r="690" ht="14.25" customHeight="1"/>
+    <row r="691" ht="14.25" customHeight="1"/>
+    <row r="692" ht="14.25" customHeight="1"/>
+    <row r="693" ht="14.25" customHeight="1"/>
+    <row r="694" ht="14.25" customHeight="1"/>
+    <row r="695" ht="14.25" customHeight="1"/>
+    <row r="696" ht="14.25" customHeight="1"/>
+    <row r="697" ht="14.25" customHeight="1"/>
+    <row r="698" ht="14.25" customHeight="1"/>
+    <row r="699" ht="14.25" customHeight="1"/>
+    <row r="700" ht="14.25" customHeight="1"/>
+    <row r="701" ht="14.25" customHeight="1"/>
+    <row r="702" ht="14.25" customHeight="1"/>
+    <row r="703" ht="14.25" customHeight="1"/>
+    <row r="704" ht="14.25" customHeight="1"/>
+    <row r="705" ht="14.25" customHeight="1"/>
+    <row r="706" ht="14.25" customHeight="1"/>
+    <row r="707" ht="14.25" customHeight="1"/>
+    <row r="708" ht="14.25" customHeight="1"/>
+    <row r="709" ht="14.25" customHeight="1"/>
+    <row r="710" ht="14.25" customHeight="1"/>
+    <row r="711" ht="14.25" customHeight="1"/>
+    <row r="712" ht="14.25" customHeight="1"/>
+    <row r="713" ht="14.25" customHeight="1"/>
+    <row r="714" ht="14.25" customHeight="1"/>
+    <row r="715" ht="14.25" customHeight="1"/>
+    <row r="716" ht="14.25" customHeight="1"/>
+    <row r="717" ht="14.25" customHeight="1"/>
+    <row r="718" ht="14.25" customHeight="1"/>
+    <row r="719" ht="14.25" customHeight="1"/>
+    <row r="720" ht="14.25" customHeight="1"/>
+    <row r="721" ht="14.25" customHeight="1"/>
+    <row r="722" ht="14.25" customHeight="1"/>
+    <row r="723" ht="14.25" customHeight="1"/>
+    <row r="724" ht="14.25" customHeight="1"/>
+    <row r="725" ht="14.25" customHeight="1"/>
+    <row r="726" ht="14.25" customHeight="1"/>
+    <row r="727" ht="14.25" customHeight="1"/>
+    <row r="728" ht="14.25" customHeight="1"/>
+    <row r="729" ht="14.25" customHeight="1"/>
+    <row r="730" ht="14.25" customHeight="1"/>
+    <row r="731" ht="14.25" customHeight="1"/>
+    <row r="732" ht="14.25" customHeight="1"/>
+    <row r="733" ht="14.25" customHeight="1"/>
+    <row r="734" ht="14.25" customHeight="1"/>
+    <row r="735" ht="14.25" customHeight="1"/>
+    <row r="736" ht="14.25" customHeight="1"/>
+    <row r="737" ht="14.25" customHeight="1"/>
+    <row r="738" ht="14.25" customHeight="1"/>
+    <row r="739" ht="14.25" customHeight="1"/>
+    <row r="740" ht="14.25" customHeight="1"/>
+    <row r="741" ht="14.25" customHeight="1"/>
+    <row r="742" ht="14.25" customHeight="1"/>
+    <row r="743" ht="14.25" customHeight="1"/>
+    <row r="744" ht="14.25" customHeight="1"/>
+    <row r="745" ht="14.25" customHeight="1"/>
+    <row r="746" ht="14.25" customHeight="1"/>
+    <row r="747" ht="14.25" customHeight="1"/>
+    <row r="748" ht="14.25" customHeight="1"/>
+    <row r="749" ht="14.25" customHeight="1"/>
+    <row r="750" ht="14.25" customHeight="1"/>
+    <row r="751" ht="14.25" customHeight="1"/>
+    <row r="752" ht="14.25" customHeight="1"/>
+    <row r="753" ht="14.25" customHeight="1"/>
+    <row r="754" ht="14.25" customHeight="1"/>
+    <row r="755" ht="14.25" customHeight="1"/>
+    <row r="756" ht="14.25" customHeight="1"/>
+    <row r="757" ht="14.25" customHeight="1"/>
+    <row r="758" ht="14.25" customHeight="1"/>
+    <row r="759" ht="14.25" customHeight="1"/>
+    <row r="760" ht="14.25" customHeight="1"/>
+    <row r="761" ht="14.25" customHeight="1"/>
+    <row r="762" ht="14.25" customHeight="1"/>
+    <row r="763" ht="14.25" customHeight="1"/>
+    <row r="764" ht="14.25" customHeight="1"/>
+    <row r="765" ht="14.25" customHeight="1"/>
+    <row r="766" ht="14.25" customHeight="1"/>
+    <row r="767" ht="14.25" customHeight="1"/>
+    <row r="768" ht="14.25" customHeight="1"/>
+    <row r="769" ht="14.25" customHeight="1"/>
+    <row r="770" ht="14.25" customHeight="1"/>
+    <row r="771" ht="14.25" customHeight="1"/>
+    <row r="772" ht="14.25" customHeight="1"/>
+    <row r="773" ht="14.25" customHeight="1"/>
+    <row r="774" ht="14.25" customHeight="1"/>
+    <row r="775" ht="14.25" customHeight="1"/>
+    <row r="776" ht="14.25" customHeight="1"/>
+    <row r="777" ht="14.25" customHeight="1"/>
+    <row r="778" ht="14.25" customHeight="1"/>
+    <row r="779" ht="14.25" customHeight="1"/>
+    <row r="780" ht="14.25" customHeight="1"/>
+    <row r="781" ht="14.25" customHeight="1"/>
+    <row r="782" ht="14.25" customHeight="1"/>
+    <row r="783" ht="14.25" customHeight="1"/>
+    <row r="784" ht="14.25" customHeight="1"/>
+    <row r="785" ht="14.25" customHeight="1"/>
+    <row r="786" ht="14.25" customHeight="1"/>
+    <row r="787" ht="14.25" customHeight="1"/>
+    <row r="788" ht="14.25" customHeight="1"/>
+    <row r="789" ht="14.25" customHeight="1"/>
+    <row r="790" ht="14.25" customHeight="1"/>
+    <row r="791" ht="14.25" customHeight="1"/>
+    <row r="792" ht="14.25" customHeight="1"/>
+    <row r="793" ht="14.25" customHeight="1"/>
+    <row r="794" ht="14.25" customHeight="1"/>
+    <row r="795" ht="14.25" customHeight="1"/>
+    <row r="796" ht="14.25" customHeight="1"/>
+    <row r="797" ht="14.25" customHeight="1"/>
+    <row r="798" ht="14.25" customHeight="1"/>
+    <row r="799" ht="14.25" customHeight="1"/>
+    <row r="800" ht="14.25" customHeight="1"/>
+    <row r="801" ht="14.25" customHeight="1"/>
+    <row r="802" ht="14.25" customHeight="1"/>
+    <row r="803" ht="14.25" customHeight="1"/>
+    <row r="804" ht="14.25" customHeight="1"/>
+    <row r="805" ht="14.25" customHeight="1"/>
+    <row r="806" ht="14.25" customHeight="1"/>
+    <row r="807" ht="14.25" customHeight="1"/>
+    <row r="808" ht="14.25" customHeight="1"/>
+    <row r="809" ht="14.25" customHeight="1"/>
+    <row r="810" ht="14.25" customHeight="1"/>
+    <row r="811" ht="14.25" customHeight="1"/>
+    <row r="812" ht="14.25" customHeight="1"/>
+    <row r="813" ht="14.25" customHeight="1"/>
+    <row r="814" ht="14.25" customHeight="1"/>
+    <row r="815" ht="14.25" customHeight="1"/>
+    <row r="816" ht="14.25" customHeight="1"/>
+    <row r="817" ht="14.25" customHeight="1"/>
+    <row r="818" ht="14.25" customHeight="1"/>
+    <row r="819" ht="14.25" customHeight="1"/>
+    <row r="820" ht="14.25" customHeight="1"/>
+    <row r="821" ht="14.25" customHeight="1"/>
+    <row r="822" ht="14.25" customHeight="1"/>
+    <row r="823" ht="14.25" customHeight="1"/>
+    <row r="824" ht="14.25" customHeight="1"/>
+    <row r="825" ht="14.25" customHeight="1"/>
+    <row r="826" ht="14.25" customHeight="1"/>
+    <row r="827" ht="14.25" customHeight="1"/>
+    <row r="828" ht="14.25" customHeight="1"/>
+    <row r="829" ht="14.25" customHeight="1"/>
+    <row r="830" ht="14.25" customHeight="1"/>
+    <row r="831" ht="14.25" customHeight="1"/>
+    <row r="832" ht="14.25" customHeight="1"/>
+    <row r="833" ht="14.25" customHeight="1"/>
+    <row r="834" ht="14.25" customHeight="1"/>
+    <row r="835" ht="14.25" customHeight="1"/>
+    <row r="836" ht="14.25" customHeight="1"/>
+    <row r="837" ht="14.25" customHeight="1"/>
+    <row r="838" ht="14.25" customHeight="1"/>
+    <row r="839" ht="14.25" customHeight="1"/>
+    <row r="840" ht="14.25" customHeight="1"/>
+    <row r="841" ht="14.25" customHeight="1"/>
+    <row r="842" ht="14.25" customHeight="1"/>
+    <row r="843" ht="14.25" customHeight="1"/>
+    <row r="844" ht="14.25" customHeight="1"/>
+    <row r="845" ht="14.25" customHeight="1"/>
+    <row r="846" ht="14.25" customHeight="1"/>
+    <row r="847" ht="14.25" customHeight="1"/>
+    <row r="848" ht="14.25" customHeight="1"/>
+    <row r="849" ht="14.25" customHeight="1"/>
+    <row r="850" ht="14.25" customHeight="1"/>
+    <row r="851" ht="14.25" customHeight="1"/>
+    <row r="852" ht="14.25" customHeight="1"/>
+    <row r="853" ht="14.25" customHeight="1"/>
+    <row r="854" ht="14.25" customHeight="1"/>
+    <row r="855" ht="14.25" customHeight="1"/>
+    <row r="856" ht="14.25" customHeight="1"/>
+    <row r="857" ht="14.25" customHeight="1"/>
+    <row r="858" ht="14.25" customHeight="1"/>
+    <row r="859" ht="14.25" customHeight="1"/>
+    <row r="860" ht="14.25" customHeight="1"/>
+    <row r="861" ht="14.25" customHeight="1"/>
+    <row r="862" ht="14.25" customHeight="1"/>
+    <row r="863" ht="14.25" customHeight="1"/>
+    <row r="864" ht="14.25" customHeight="1"/>
+    <row r="865" ht="14.25" customHeight="1"/>
+    <row r="866" ht="14.25" customHeight="1"/>
+    <row r="867" ht="14.25" customHeight="1"/>
+    <row r="868" ht="14.25" customHeight="1"/>
+    <row r="869" ht="14.25" customHeight="1"/>
+    <row r="870" ht="14.25" customHeight="1"/>
+    <row r="871" ht="14.25" customHeight="1"/>
+    <row r="872" ht="14.25" customHeight="1"/>
+    <row r="873" ht="14.25" customHeight="1"/>
+    <row r="874" ht="14.25" customHeight="1"/>
+    <row r="875" ht="14.25" customHeight="1"/>
+    <row r="876" ht="14.25" customHeight="1"/>
+    <row r="877" ht="14.25" customHeight="1"/>
+    <row r="878" ht="14.25" customHeight="1"/>
+    <row r="879" ht="14.25" customHeight="1"/>
+    <row r="880" ht="14.25" customHeight="1"/>
+    <row r="881" ht="14.25" customHeight="1"/>
+    <row r="882" ht="14.25" customHeight="1"/>
+    <row r="883" ht="14.25" customHeight="1"/>
+    <row r="884" ht="14.25" customHeight="1"/>
+    <row r="885" ht="14.25" customHeight="1"/>
+    <row r="886" ht="14.25" customHeight="1"/>
+    <row r="887" ht="14.25" customHeight="1"/>
+    <row r="888" ht="14.25" customHeight="1"/>
+    <row r="889" ht="14.25" customHeight="1"/>
+    <row r="890" ht="14.25" customHeight="1"/>
+    <row r="891" ht="14.25" customHeight="1"/>
+    <row r="892" ht="14.25" customHeight="1"/>
+    <row r="893" ht="14.25" customHeight="1"/>
+    <row r="894" ht="14.25" customHeight="1"/>
+    <row r="895" ht="14.25" customHeight="1"/>
+    <row r="896" ht="14.25" customHeight="1"/>
+    <row r="897" ht="14.25" customHeight="1"/>
+    <row r="898" ht="14.25" customHeight="1"/>
+    <row r="899" ht="14.25" customHeight="1"/>
+    <row r="900" ht="14.25" customHeight="1"/>
+    <row r="901" ht="14.25" customHeight="1"/>
+    <row r="902" ht="14.25" customHeight="1"/>
+    <row r="903" ht="14.25" customHeight="1"/>
+    <row r="904" ht="14.25" customHeight="1"/>
+    <row r="905" ht="14.25" customHeight="1"/>
+    <row r="906" ht="14.25" customHeight="1"/>
+    <row r="907" ht="14.25" customHeight="1"/>
+    <row r="908" ht="14.25" customHeight="1"/>
+    <row r="909" ht="14.25" customHeight="1"/>
+    <row r="910" ht="14.25" customHeight="1"/>
+    <row r="911" ht="14.25" customHeight="1"/>
+    <row r="912" ht="14.25" customHeight="1"/>
+    <row r="913" ht="14.25" customHeight="1"/>
+    <row r="914" ht="14.25" customHeight="1"/>
+    <row r="915" ht="14.25" customHeight="1"/>
+    <row r="916" ht="14.25" customHeight="1"/>
+    <row r="917" ht="14.25" customHeight="1"/>
+    <row r="918" ht="14.25" customHeight="1"/>
+    <row r="919" ht="14.25" customHeight="1"/>
+    <row r="920" ht="14.25" customHeight="1"/>
+    <row r="921" ht="14.25" customHeight="1"/>
+    <row r="922" ht="14.25" customHeight="1"/>
+    <row r="923" ht="14.25" customHeight="1"/>
+    <row r="924" ht="14.25" customHeight="1"/>
+    <row r="925" ht="14.25" customHeight="1"/>
+    <row r="926" ht="14.25" customHeight="1"/>
+    <row r="927" ht="14.25" customHeight="1"/>
+    <row r="928" ht="14.25" customHeight="1"/>
+    <row r="929" ht="14.25" customHeight="1"/>
+    <row r="930" ht="14.25" customHeight="1"/>
+    <row r="931" ht="14.25" customHeight="1"/>
+    <row r="932" ht="14.25" customHeight="1"/>
+    <row r="933" ht="14.25" customHeight="1"/>
+    <row r="934" ht="14.25" customHeight="1"/>
+    <row r="935" ht="14.25" customHeight="1"/>
+    <row r="936" ht="14.25" customHeight="1"/>
+    <row r="937" ht="14.25" customHeight="1"/>
+    <row r="938" ht="14.25" customHeight="1"/>
+    <row r="939" ht="14.25" customHeight="1"/>
+    <row r="940" ht="14.25" customHeight="1"/>
+    <row r="941" ht="14.25" customHeight="1"/>
+    <row r="942" ht="14.25" customHeight="1"/>
+    <row r="943" ht="14.25" customHeight="1"/>
+    <row r="944" ht="14.25" customHeight="1"/>
+    <row r="945" ht="14.25" customHeight="1"/>
+    <row r="946" ht="14.25" customHeight="1"/>
+    <row r="947" ht="14.25" customHeight="1"/>
+    <row r="948" ht="14.25" customHeight="1"/>
+    <row r="949" ht="14.25" customHeight="1"/>
+    <row r="950" ht="14.25" customHeight="1"/>
+    <row r="951" ht="14.25" customHeight="1"/>
+    <row r="952" ht="14.25" customHeight="1"/>
+    <row r="953" ht="14.25" customHeight="1"/>
+    <row r="954" ht="14.25" customHeight="1"/>
+    <row r="955" ht="14.25" customHeight="1"/>
+    <row r="956" ht="14.25" customHeight="1"/>
+    <row r="957" ht="14.25" customHeight="1"/>
+    <row r="958" ht="14.25" customHeight="1"/>
+    <row r="959" ht="14.25" customHeight="1"/>
+    <row r="960" ht="14.25" customHeight="1"/>
+    <row r="961" ht="14.25" customHeight="1"/>
+    <row r="962" ht="14.25" customHeight="1"/>
+    <row r="963" ht="14.25" customHeight="1"/>
+    <row r="964" ht="14.25" customHeight="1"/>
+    <row r="965" ht="14.25" customHeight="1"/>
+    <row r="966" ht="14.25" customHeight="1"/>
+    <row r="967" ht="14.25" customHeight="1"/>
+    <row r="968" ht="14.25" customHeight="1"/>
+    <row r="969" ht="14.25" customHeight="1"/>
+    <row r="970" ht="14.25" customHeight="1"/>
+    <row r="971" ht="14.25" customHeight="1"/>
+    <row r="972" ht="14.25" customHeight="1"/>
+    <row r="973" ht="14.25" customHeight="1"/>
+    <row r="974" ht="14.25" customHeight="1"/>
+    <row r="975" ht="14.25" customHeight="1"/>
+    <row r="976" ht="14.25" customHeight="1"/>
+    <row r="977" ht="14.25" customHeight="1"/>
+    <row r="978" ht="14.25" customHeight="1"/>
+    <row r="979" ht="14.25" customHeight="1"/>
+    <row r="980" ht="14.25" customHeight="1"/>
+    <row r="981" ht="14.25" customHeight="1"/>
+    <row r="982" ht="14.25" customHeight="1"/>
+    <row r="983" ht="14.25" customHeight="1"/>
+    <row r="984" ht="14.25" customHeight="1"/>
+    <row r="985" ht="14.25" customHeight="1"/>
+    <row r="986" ht="14.25" customHeight="1"/>
+    <row r="987" ht="14.25" customHeight="1"/>
+    <row r="988" ht="14.25" customHeight="1"/>
+    <row r="989" ht="14.25" customHeight="1"/>
+    <row r="990" ht="14.25" customHeight="1"/>
+    <row r="991" ht="14.25" customHeight="1"/>
+    <row r="992" ht="14.25" customHeight="1"/>
+    <row r="993" ht="14.25" customHeight="1"/>
+    <row r="994" ht="14.25" customHeight="1"/>
+    <row r="995" ht="14.25" customHeight="1"/>
+    <row r="996" ht="14.25" customHeight="1"/>
+    <row r="997" ht="14.25" customHeight="1"/>
+    <row r="998" ht="14.25" customHeight="1"/>
+    <row r="999" ht="14.25" customHeight="1"/>
+    <row r="1000" ht="14.25" customHeight="1"/>
+    <row r="1001" ht="14.25" customHeight="1"/>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="B3:F3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <pageSetup orientation="landscape"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0" topLeftCell="A4"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.63" defaultRowHeight="15" customHeight="1"/>
+  <cols>
+    <col min="1" max="1" width="0.88" customWidth="1"/>
+    <col min="2" max="2" width="44.63" customWidth="1"/>
+    <col min="3" max="3" width="30.38" customWidth="1"/>
+    <col min="4" max="4" width="10.63" customWidth="1"/>
+    <col min="5" max="5" width="33.5" customWidth="1"/>
+    <col min="6" max="6" width="20.75" customWidth="1"/>
+    <col min="7" max="7" width="62.88" customWidth="1"/>
+    <col min="8" max="26" width="10.63" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="4.5" customHeight="1"/>
+    <row r="2" ht="120" customHeight="1">
+      <c r="B2" s="1"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+    </row>
+    <row r="3" ht="30" customHeight="1">
+      <c r="B3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="5"/>
+    </row>
+    <row r="4" ht="30" customHeight="1">
+      <c r="B4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" ht="27" customHeight="1">
+      <c r="B5" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D5" s="9"/>
+      <c r="E5" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" ht="25.5" customHeight="1">
+      <c r="B6" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6" s="9"/>
+      <c r="E6" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" ht="28.5" customHeight="1">
+      <c r="B7" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="D7" s="9"/>
+      <c r="E7" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" ht="28.5" customHeight="1">
+      <c r="B8" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" s="9"/>
+      <c r="E8" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>57</v>
+      </c>
+    </row>
     <row r="17" ht="14.25" customHeight="1"/>
     <row r="18" ht="14.25" customHeight="1"/>
     <row r="19" ht="14.25" customHeight="1"/>
@@ -2963,1139 +4089,7 @@
     <mergeCell ref="B2:F2"/>
     <mergeCell ref="B3:F3"/>
   </mergeCells>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <sheetPr>
-    <pageSetUpPr/>
-  </sheetPr>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
-  <cols>
-    <col customWidth="1" min="1" max="1" width="0.88"/>
-    <col customWidth="1" min="2" max="2" width="44.63"/>
-    <col customWidth="1" min="3" max="3" width="30.38"/>
-    <col customWidth="1" min="4" max="4" width="10.63"/>
-    <col customWidth="1" min="5" max="5" width="33.5"/>
-    <col customWidth="1" min="6" max="6" width="20.75"/>
-    <col customWidth="1" min="7" max="7" width="62.88"/>
-    <col customWidth="1" min="8" max="26" width="10.63"/>
-  </cols>
-  <sheetData>
-    <row r="1" ht="4.5" customHeight="1"/>
-    <row r="2" ht="120.0" customHeight="1">
-      <c r="B2" s="1"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-    </row>
-    <row r="3" ht="30.0" customHeight="1">
-      <c r="B3" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="5"/>
-    </row>
-    <row r="4" ht="30.0" customHeight="1">
-      <c r="B4" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" ht="27.0" customHeight="1">
-      <c r="B5" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="C5" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="D5" s="9"/>
-      <c r="E5" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="F5" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="G5" s="14" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" ht="25.5" customHeight="1">
-      <c r="B6" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="C6" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="F6" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="G6" s="14" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7" ht="28.5" customHeight="1">
-      <c r="B7" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="C7" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="D7" s="9"/>
-      <c r="E7" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="F7" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="G7" s="14" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="8" ht="28.5" customHeight="1">
-      <c r="B8" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="D8" s="9"/>
-      <c r="E8" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="F8" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="G8" s="14" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="9" ht="15.0" customHeight="1"/>
-    <row r="10" ht="15.0" customHeight="1"/>
-    <row r="11" ht="15.0" customHeight="1"/>
-    <row r="12" ht="15.0" customHeight="1"/>
-    <row r="13" ht="15.0" customHeight="1"/>
-    <row r="14" ht="15.0" customHeight="1"/>
-    <row r="15" ht="15.0" customHeight="1"/>
-    <row r="16" ht="15.0" customHeight="1"/>
-    <row r="17" ht="14.25" customHeight="1"/>
-    <row r="18" ht="14.25" customHeight="1"/>
-    <row r="19" ht="14.25" customHeight="1"/>
-    <row r="20" ht="14.25" customHeight="1"/>
-    <row r="21" ht="14.25" customHeight="1"/>
-    <row r="22" ht="14.25" customHeight="1"/>
-    <row r="23" ht="14.25" customHeight="1"/>
-    <row r="24" ht="14.25" customHeight="1"/>
-    <row r="25" ht="14.25" customHeight="1"/>
-    <row r="26" ht="14.25" customHeight="1"/>
-    <row r="27" ht="14.25" customHeight="1"/>
-    <row r="28" ht="14.25" customHeight="1"/>
-    <row r="29" ht="14.25" customHeight="1"/>
-    <row r="30" ht="14.25" customHeight="1"/>
-    <row r="31" ht="14.25" customHeight="1"/>
-    <row r="32" ht="14.25" customHeight="1"/>
-    <row r="33" ht="14.25" customHeight="1"/>
-    <row r="34" ht="14.25" customHeight="1"/>
-    <row r="35" ht="14.25" customHeight="1"/>
-    <row r="36" ht="14.25" customHeight="1"/>
-    <row r="37" ht="14.25" customHeight="1"/>
-    <row r="38" ht="14.25" customHeight="1"/>
-    <row r="39" ht="14.25" customHeight="1"/>
-    <row r="40" ht="14.25" customHeight="1"/>
-    <row r="41" ht="14.25" customHeight="1"/>
-    <row r="42" ht="14.25" customHeight="1"/>
-    <row r="43" ht="14.25" customHeight="1"/>
-    <row r="44" ht="14.25" customHeight="1"/>
-    <row r="45" ht="14.25" customHeight="1"/>
-    <row r="46" ht="14.25" customHeight="1"/>
-    <row r="47" ht="14.25" customHeight="1"/>
-    <row r="48" ht="14.25" customHeight="1"/>
-    <row r="49" ht="14.25" customHeight="1"/>
-    <row r="50" ht="14.25" customHeight="1"/>
-    <row r="51" ht="14.25" customHeight="1"/>
-    <row r="52" ht="14.25" customHeight="1"/>
-    <row r="53" ht="14.25" customHeight="1"/>
-    <row r="54" ht="14.25" customHeight="1"/>
-    <row r="55" ht="14.25" customHeight="1"/>
-    <row r="56" ht="14.25" customHeight="1"/>
-    <row r="57" ht="14.25" customHeight="1"/>
-    <row r="58" ht="14.25" customHeight="1"/>
-    <row r="59" ht="14.25" customHeight="1"/>
-    <row r="60" ht="14.25" customHeight="1"/>
-    <row r="61" ht="14.25" customHeight="1"/>
-    <row r="62" ht="14.25" customHeight="1"/>
-    <row r="63" ht="14.25" customHeight="1"/>
-    <row r="64" ht="14.25" customHeight="1"/>
-    <row r="65" ht="14.25" customHeight="1"/>
-    <row r="66" ht="14.25" customHeight="1"/>
-    <row r="67" ht="14.25" customHeight="1"/>
-    <row r="68" ht="14.25" customHeight="1"/>
-    <row r="69" ht="14.25" customHeight="1"/>
-    <row r="70" ht="14.25" customHeight="1"/>
-    <row r="71" ht="14.25" customHeight="1"/>
-    <row r="72" ht="14.25" customHeight="1"/>
-    <row r="73" ht="14.25" customHeight="1"/>
-    <row r="74" ht="14.25" customHeight="1"/>
-    <row r="75" ht="14.25" customHeight="1"/>
-    <row r="76" ht="14.25" customHeight="1"/>
-    <row r="77" ht="14.25" customHeight="1"/>
-    <row r="78" ht="14.25" customHeight="1"/>
-    <row r="79" ht="14.25" customHeight="1"/>
-    <row r="80" ht="14.25" customHeight="1"/>
-    <row r="81" ht="14.25" customHeight="1"/>
-    <row r="82" ht="14.25" customHeight="1"/>
-    <row r="83" ht="14.25" customHeight="1"/>
-    <row r="84" ht="14.25" customHeight="1"/>
-    <row r="85" ht="14.25" customHeight="1"/>
-    <row r="86" ht="14.25" customHeight="1"/>
-    <row r="87" ht="14.25" customHeight="1"/>
-    <row r="88" ht="14.25" customHeight="1"/>
-    <row r="89" ht="14.25" customHeight="1"/>
-    <row r="90" ht="14.25" customHeight="1"/>
-    <row r="91" ht="14.25" customHeight="1"/>
-    <row r="92" ht="14.25" customHeight="1"/>
-    <row r="93" ht="14.25" customHeight="1"/>
-    <row r="94" ht="14.25" customHeight="1"/>
-    <row r="95" ht="14.25" customHeight="1"/>
-    <row r="96" ht="14.25" customHeight="1"/>
-    <row r="97" ht="14.25" customHeight="1"/>
-    <row r="98" ht="14.25" customHeight="1"/>
-    <row r="99" ht="14.25" customHeight="1"/>
-    <row r="100" ht="14.25" customHeight="1"/>
-    <row r="101" ht="14.25" customHeight="1"/>
-    <row r="102" ht="14.25" customHeight="1"/>
-    <row r="103" ht="14.25" customHeight="1"/>
-    <row r="104" ht="14.25" customHeight="1"/>
-    <row r="105" ht="14.25" customHeight="1"/>
-    <row r="106" ht="14.25" customHeight="1"/>
-    <row r="107" ht="14.25" customHeight="1"/>
-    <row r="108" ht="14.25" customHeight="1"/>
-    <row r="109" ht="14.25" customHeight="1"/>
-    <row r="110" ht="14.25" customHeight="1"/>
-    <row r="111" ht="14.25" customHeight="1"/>
-    <row r="112" ht="14.25" customHeight="1"/>
-    <row r="113" ht="14.25" customHeight="1"/>
-    <row r="114" ht="14.25" customHeight="1"/>
-    <row r="115" ht="14.25" customHeight="1"/>
-    <row r="116" ht="14.25" customHeight="1"/>
-    <row r="117" ht="14.25" customHeight="1"/>
-    <row r="118" ht="14.25" customHeight="1"/>
-    <row r="119" ht="14.25" customHeight="1"/>
-    <row r="120" ht="14.25" customHeight="1"/>
-    <row r="121" ht="14.25" customHeight="1"/>
-    <row r="122" ht="14.25" customHeight="1"/>
-    <row r="123" ht="14.25" customHeight="1"/>
-    <row r="124" ht="14.25" customHeight="1"/>
-    <row r="125" ht="14.25" customHeight="1"/>
-    <row r="126" ht="14.25" customHeight="1"/>
-    <row r="127" ht="14.25" customHeight="1"/>
-    <row r="128" ht="14.25" customHeight="1"/>
-    <row r="129" ht="14.25" customHeight="1"/>
-    <row r="130" ht="14.25" customHeight="1"/>
-    <row r="131" ht="14.25" customHeight="1"/>
-    <row r="132" ht="14.25" customHeight="1"/>
-    <row r="133" ht="14.25" customHeight="1"/>
-    <row r="134" ht="14.25" customHeight="1"/>
-    <row r="135" ht="14.25" customHeight="1"/>
-    <row r="136" ht="14.25" customHeight="1"/>
-    <row r="137" ht="14.25" customHeight="1"/>
-    <row r="138" ht="14.25" customHeight="1"/>
-    <row r="139" ht="14.25" customHeight="1"/>
-    <row r="140" ht="14.25" customHeight="1"/>
-    <row r="141" ht="14.25" customHeight="1"/>
-    <row r="142" ht="14.25" customHeight="1"/>
-    <row r="143" ht="14.25" customHeight="1"/>
-    <row r="144" ht="14.25" customHeight="1"/>
-    <row r="145" ht="14.25" customHeight="1"/>
-    <row r="146" ht="14.25" customHeight="1"/>
-    <row r="147" ht="14.25" customHeight="1"/>
-    <row r="148" ht="14.25" customHeight="1"/>
-    <row r="149" ht="14.25" customHeight="1"/>
-    <row r="150" ht="14.25" customHeight="1"/>
-    <row r="151" ht="14.25" customHeight="1"/>
-    <row r="152" ht="14.25" customHeight="1"/>
-    <row r="153" ht="14.25" customHeight="1"/>
-    <row r="154" ht="14.25" customHeight="1"/>
-    <row r="155" ht="14.25" customHeight="1"/>
-    <row r="156" ht="14.25" customHeight="1"/>
-    <row r="157" ht="14.25" customHeight="1"/>
-    <row r="158" ht="14.25" customHeight="1"/>
-    <row r="159" ht="14.25" customHeight="1"/>
-    <row r="160" ht="14.25" customHeight="1"/>
-    <row r="161" ht="14.25" customHeight="1"/>
-    <row r="162" ht="14.25" customHeight="1"/>
-    <row r="163" ht="14.25" customHeight="1"/>
-    <row r="164" ht="14.25" customHeight="1"/>
-    <row r="165" ht="14.25" customHeight="1"/>
-    <row r="166" ht="14.25" customHeight="1"/>
-    <row r="167" ht="14.25" customHeight="1"/>
-    <row r="168" ht="14.25" customHeight="1"/>
-    <row r="169" ht="14.25" customHeight="1"/>
-    <row r="170" ht="14.25" customHeight="1"/>
-    <row r="171" ht="14.25" customHeight="1"/>
-    <row r="172" ht="14.25" customHeight="1"/>
-    <row r="173" ht="14.25" customHeight="1"/>
-    <row r="174" ht="14.25" customHeight="1"/>
-    <row r="175" ht="14.25" customHeight="1"/>
-    <row r="176" ht="14.25" customHeight="1"/>
-    <row r="177" ht="14.25" customHeight="1"/>
-    <row r="178" ht="14.25" customHeight="1"/>
-    <row r="179" ht="14.25" customHeight="1"/>
-    <row r="180" ht="14.25" customHeight="1"/>
-    <row r="181" ht="14.25" customHeight="1"/>
-    <row r="182" ht="14.25" customHeight="1"/>
-    <row r="183" ht="14.25" customHeight="1"/>
-    <row r="184" ht="14.25" customHeight="1"/>
-    <row r="185" ht="14.25" customHeight="1"/>
-    <row r="186" ht="14.25" customHeight="1"/>
-    <row r="187" ht="14.25" customHeight="1"/>
-    <row r="188" ht="14.25" customHeight="1"/>
-    <row r="189" ht="14.25" customHeight="1"/>
-    <row r="190" ht="14.25" customHeight="1"/>
-    <row r="191" ht="14.25" customHeight="1"/>
-    <row r="192" ht="14.25" customHeight="1"/>
-    <row r="193" ht="14.25" customHeight="1"/>
-    <row r="194" ht="14.25" customHeight="1"/>
-    <row r="195" ht="14.25" customHeight="1"/>
-    <row r="196" ht="14.25" customHeight="1"/>
-    <row r="197" ht="14.25" customHeight="1"/>
-    <row r="198" ht="14.25" customHeight="1"/>
-    <row r="199" ht="14.25" customHeight="1"/>
-    <row r="200" ht="14.25" customHeight="1"/>
-    <row r="201" ht="14.25" customHeight="1"/>
-    <row r="202" ht="14.25" customHeight="1"/>
-    <row r="203" ht="14.25" customHeight="1"/>
-    <row r="204" ht="14.25" customHeight="1"/>
-    <row r="205" ht="14.25" customHeight="1"/>
-    <row r="206" ht="14.25" customHeight="1"/>
-    <row r="207" ht="14.25" customHeight="1"/>
-    <row r="208" ht="14.25" customHeight="1"/>
-    <row r="209" ht="14.25" customHeight="1"/>
-    <row r="210" ht="14.25" customHeight="1"/>
-    <row r="211" ht="14.25" customHeight="1"/>
-    <row r="212" ht="14.25" customHeight="1"/>
-    <row r="213" ht="14.25" customHeight="1"/>
-    <row r="214" ht="14.25" customHeight="1"/>
-    <row r="215" ht="14.25" customHeight="1"/>
-    <row r="216" ht="14.25" customHeight="1"/>
-    <row r="217" ht="14.25" customHeight="1"/>
-    <row r="218" ht="14.25" customHeight="1"/>
-    <row r="219" ht="14.25" customHeight="1"/>
-    <row r="220" ht="14.25" customHeight="1"/>
-    <row r="221" ht="14.25" customHeight="1"/>
-    <row r="222" ht="14.25" customHeight="1"/>
-    <row r="223" ht="14.25" customHeight="1"/>
-    <row r="224" ht="14.25" customHeight="1"/>
-    <row r="225" ht="14.25" customHeight="1"/>
-    <row r="226" ht="14.25" customHeight="1"/>
-    <row r="227" ht="14.25" customHeight="1"/>
-    <row r="228" ht="14.25" customHeight="1"/>
-    <row r="229" ht="14.25" customHeight="1"/>
-    <row r="230" ht="14.25" customHeight="1"/>
-    <row r="231" ht="14.25" customHeight="1"/>
-    <row r="232" ht="14.25" customHeight="1"/>
-    <row r="233" ht="14.25" customHeight="1"/>
-    <row r="234" ht="14.25" customHeight="1"/>
-    <row r="235" ht="14.25" customHeight="1"/>
-    <row r="236" ht="14.25" customHeight="1"/>
-    <row r="237" ht="14.25" customHeight="1"/>
-    <row r="238" ht="14.25" customHeight="1"/>
-    <row r="239" ht="14.25" customHeight="1"/>
-    <row r="240" ht="14.25" customHeight="1"/>
-    <row r="241" ht="14.25" customHeight="1"/>
-    <row r="242" ht="14.25" customHeight="1"/>
-    <row r="243" ht="14.25" customHeight="1"/>
-    <row r="244" ht="14.25" customHeight="1"/>
-    <row r="245" ht="14.25" customHeight="1"/>
-    <row r="246" ht="14.25" customHeight="1"/>
-    <row r="247" ht="14.25" customHeight="1"/>
-    <row r="248" ht="14.25" customHeight="1"/>
-    <row r="249" ht="14.25" customHeight="1"/>
-    <row r="250" ht="14.25" customHeight="1"/>
-    <row r="251" ht="14.25" customHeight="1"/>
-    <row r="252" ht="14.25" customHeight="1"/>
-    <row r="253" ht="14.25" customHeight="1"/>
-    <row r="254" ht="14.25" customHeight="1"/>
-    <row r="255" ht="14.25" customHeight="1"/>
-    <row r="256" ht="14.25" customHeight="1"/>
-    <row r="257" ht="14.25" customHeight="1"/>
-    <row r="258" ht="14.25" customHeight="1"/>
-    <row r="259" ht="14.25" customHeight="1"/>
-    <row r="260" ht="14.25" customHeight="1"/>
-    <row r="261" ht="14.25" customHeight="1"/>
-    <row r="262" ht="14.25" customHeight="1"/>
-    <row r="263" ht="14.25" customHeight="1"/>
-    <row r="264" ht="14.25" customHeight="1"/>
-    <row r="265" ht="14.25" customHeight="1"/>
-    <row r="266" ht="14.25" customHeight="1"/>
-    <row r="267" ht="14.25" customHeight="1"/>
-    <row r="268" ht="14.25" customHeight="1"/>
-    <row r="269" ht="14.25" customHeight="1"/>
-    <row r="270" ht="14.25" customHeight="1"/>
-    <row r="271" ht="14.25" customHeight="1"/>
-    <row r="272" ht="14.25" customHeight="1"/>
-    <row r="273" ht="14.25" customHeight="1"/>
-    <row r="274" ht="14.25" customHeight="1"/>
-    <row r="275" ht="14.25" customHeight="1"/>
-    <row r="276" ht="14.25" customHeight="1"/>
-    <row r="277" ht="14.25" customHeight="1"/>
-    <row r="278" ht="14.25" customHeight="1"/>
-    <row r="279" ht="14.25" customHeight="1"/>
-    <row r="280" ht="14.25" customHeight="1"/>
-    <row r="281" ht="14.25" customHeight="1"/>
-    <row r="282" ht="14.25" customHeight="1"/>
-    <row r="283" ht="14.25" customHeight="1"/>
-    <row r="284" ht="14.25" customHeight="1"/>
-    <row r="285" ht="14.25" customHeight="1"/>
-    <row r="286" ht="14.25" customHeight="1"/>
-    <row r="287" ht="14.25" customHeight="1"/>
-    <row r="288" ht="14.25" customHeight="1"/>
-    <row r="289" ht="14.25" customHeight="1"/>
-    <row r="290" ht="14.25" customHeight="1"/>
-    <row r="291" ht="14.25" customHeight="1"/>
-    <row r="292" ht="14.25" customHeight="1"/>
-    <row r="293" ht="14.25" customHeight="1"/>
-    <row r="294" ht="14.25" customHeight="1"/>
-    <row r="295" ht="14.25" customHeight="1"/>
-    <row r="296" ht="14.25" customHeight="1"/>
-    <row r="297" ht="14.25" customHeight="1"/>
-    <row r="298" ht="14.25" customHeight="1"/>
-    <row r="299" ht="14.25" customHeight="1"/>
-    <row r="300" ht="14.25" customHeight="1"/>
-    <row r="301" ht="14.25" customHeight="1"/>
-    <row r="302" ht="14.25" customHeight="1"/>
-    <row r="303" ht="14.25" customHeight="1"/>
-    <row r="304" ht="14.25" customHeight="1"/>
-    <row r="305" ht="14.25" customHeight="1"/>
-    <row r="306" ht="14.25" customHeight="1"/>
-    <row r="307" ht="14.25" customHeight="1"/>
-    <row r="308" ht="14.25" customHeight="1"/>
-    <row r="309" ht="14.25" customHeight="1"/>
-    <row r="310" ht="14.25" customHeight="1"/>
-    <row r="311" ht="14.25" customHeight="1"/>
-    <row r="312" ht="14.25" customHeight="1"/>
-    <row r="313" ht="14.25" customHeight="1"/>
-    <row r="314" ht="14.25" customHeight="1"/>
-    <row r="315" ht="14.25" customHeight="1"/>
-    <row r="316" ht="14.25" customHeight="1"/>
-    <row r="317" ht="14.25" customHeight="1"/>
-    <row r="318" ht="14.25" customHeight="1"/>
-    <row r="319" ht="14.25" customHeight="1"/>
-    <row r="320" ht="14.25" customHeight="1"/>
-    <row r="321" ht="14.25" customHeight="1"/>
-    <row r="322" ht="14.25" customHeight="1"/>
-    <row r="323" ht="14.25" customHeight="1"/>
-    <row r="324" ht="14.25" customHeight="1"/>
-    <row r="325" ht="14.25" customHeight="1"/>
-    <row r="326" ht="14.25" customHeight="1"/>
-    <row r="327" ht="14.25" customHeight="1"/>
-    <row r="328" ht="14.25" customHeight="1"/>
-    <row r="329" ht="14.25" customHeight="1"/>
-    <row r="330" ht="14.25" customHeight="1"/>
-    <row r="331" ht="14.25" customHeight="1"/>
-    <row r="332" ht="14.25" customHeight="1"/>
-    <row r="333" ht="14.25" customHeight="1"/>
-    <row r="334" ht="14.25" customHeight="1"/>
-    <row r="335" ht="14.25" customHeight="1"/>
-    <row r="336" ht="14.25" customHeight="1"/>
-    <row r="337" ht="14.25" customHeight="1"/>
-    <row r="338" ht="14.25" customHeight="1"/>
-    <row r="339" ht="14.25" customHeight="1"/>
-    <row r="340" ht="14.25" customHeight="1"/>
-    <row r="341" ht="14.25" customHeight="1"/>
-    <row r="342" ht="14.25" customHeight="1"/>
-    <row r="343" ht="14.25" customHeight="1"/>
-    <row r="344" ht="14.25" customHeight="1"/>
-    <row r="345" ht="14.25" customHeight="1"/>
-    <row r="346" ht="14.25" customHeight="1"/>
-    <row r="347" ht="14.25" customHeight="1"/>
-    <row r="348" ht="14.25" customHeight="1"/>
-    <row r="349" ht="14.25" customHeight="1"/>
-    <row r="350" ht="14.25" customHeight="1"/>
-    <row r="351" ht="14.25" customHeight="1"/>
-    <row r="352" ht="14.25" customHeight="1"/>
-    <row r="353" ht="14.25" customHeight="1"/>
-    <row r="354" ht="14.25" customHeight="1"/>
-    <row r="355" ht="14.25" customHeight="1"/>
-    <row r="356" ht="14.25" customHeight="1"/>
-    <row r="357" ht="14.25" customHeight="1"/>
-    <row r="358" ht="14.25" customHeight="1"/>
-    <row r="359" ht="14.25" customHeight="1"/>
-    <row r="360" ht="14.25" customHeight="1"/>
-    <row r="361" ht="14.25" customHeight="1"/>
-    <row r="362" ht="14.25" customHeight="1"/>
-    <row r="363" ht="14.25" customHeight="1"/>
-    <row r="364" ht="14.25" customHeight="1"/>
-    <row r="365" ht="14.25" customHeight="1"/>
-    <row r="366" ht="14.25" customHeight="1"/>
-    <row r="367" ht="14.25" customHeight="1"/>
-    <row r="368" ht="14.25" customHeight="1"/>
-    <row r="369" ht="14.25" customHeight="1"/>
-    <row r="370" ht="14.25" customHeight="1"/>
-    <row r="371" ht="14.25" customHeight="1"/>
-    <row r="372" ht="14.25" customHeight="1"/>
-    <row r="373" ht="14.25" customHeight="1"/>
-    <row r="374" ht="14.25" customHeight="1"/>
-    <row r="375" ht="14.25" customHeight="1"/>
-    <row r="376" ht="14.25" customHeight="1"/>
-    <row r="377" ht="14.25" customHeight="1"/>
-    <row r="378" ht="14.25" customHeight="1"/>
-    <row r="379" ht="14.25" customHeight="1"/>
-    <row r="380" ht="14.25" customHeight="1"/>
-    <row r="381" ht="14.25" customHeight="1"/>
-    <row r="382" ht="14.25" customHeight="1"/>
-    <row r="383" ht="14.25" customHeight="1"/>
-    <row r="384" ht="14.25" customHeight="1"/>
-    <row r="385" ht="14.25" customHeight="1"/>
-    <row r="386" ht="14.25" customHeight="1"/>
-    <row r="387" ht="14.25" customHeight="1"/>
-    <row r="388" ht="14.25" customHeight="1"/>
-    <row r="389" ht="14.25" customHeight="1"/>
-    <row r="390" ht="14.25" customHeight="1"/>
-    <row r="391" ht="14.25" customHeight="1"/>
-    <row r="392" ht="14.25" customHeight="1"/>
-    <row r="393" ht="14.25" customHeight="1"/>
-    <row r="394" ht="14.25" customHeight="1"/>
-    <row r="395" ht="14.25" customHeight="1"/>
-    <row r="396" ht="14.25" customHeight="1"/>
-    <row r="397" ht="14.25" customHeight="1"/>
-    <row r="398" ht="14.25" customHeight="1"/>
-    <row r="399" ht="14.25" customHeight="1"/>
-    <row r="400" ht="14.25" customHeight="1"/>
-    <row r="401" ht="14.25" customHeight="1"/>
-    <row r="402" ht="14.25" customHeight="1"/>
-    <row r="403" ht="14.25" customHeight="1"/>
-    <row r="404" ht="14.25" customHeight="1"/>
-    <row r="405" ht="14.25" customHeight="1"/>
-    <row r="406" ht="14.25" customHeight="1"/>
-    <row r="407" ht="14.25" customHeight="1"/>
-    <row r="408" ht="14.25" customHeight="1"/>
-    <row r="409" ht="14.25" customHeight="1"/>
-    <row r="410" ht="14.25" customHeight="1"/>
-    <row r="411" ht="14.25" customHeight="1"/>
-    <row r="412" ht="14.25" customHeight="1"/>
-    <row r="413" ht="14.25" customHeight="1"/>
-    <row r="414" ht="14.25" customHeight="1"/>
-    <row r="415" ht="14.25" customHeight="1"/>
-    <row r="416" ht="14.25" customHeight="1"/>
-    <row r="417" ht="14.25" customHeight="1"/>
-    <row r="418" ht="14.25" customHeight="1"/>
-    <row r="419" ht="14.25" customHeight="1"/>
-    <row r="420" ht="14.25" customHeight="1"/>
-    <row r="421" ht="14.25" customHeight="1"/>
-    <row r="422" ht="14.25" customHeight="1"/>
-    <row r="423" ht="14.25" customHeight="1"/>
-    <row r="424" ht="14.25" customHeight="1"/>
-    <row r="425" ht="14.25" customHeight="1"/>
-    <row r="426" ht="14.25" customHeight="1"/>
-    <row r="427" ht="14.25" customHeight="1"/>
-    <row r="428" ht="14.25" customHeight="1"/>
-    <row r="429" ht="14.25" customHeight="1"/>
-    <row r="430" ht="14.25" customHeight="1"/>
-    <row r="431" ht="14.25" customHeight="1"/>
-    <row r="432" ht="14.25" customHeight="1"/>
-    <row r="433" ht="14.25" customHeight="1"/>
-    <row r="434" ht="14.25" customHeight="1"/>
-    <row r="435" ht="14.25" customHeight="1"/>
-    <row r="436" ht="14.25" customHeight="1"/>
-    <row r="437" ht="14.25" customHeight="1"/>
-    <row r="438" ht="14.25" customHeight="1"/>
-    <row r="439" ht="14.25" customHeight="1"/>
-    <row r="440" ht="14.25" customHeight="1"/>
-    <row r="441" ht="14.25" customHeight="1"/>
-    <row r="442" ht="14.25" customHeight="1"/>
-    <row r="443" ht="14.25" customHeight="1"/>
-    <row r="444" ht="14.25" customHeight="1"/>
-    <row r="445" ht="14.25" customHeight="1"/>
-    <row r="446" ht="14.25" customHeight="1"/>
-    <row r="447" ht="14.25" customHeight="1"/>
-    <row r="448" ht="14.25" customHeight="1"/>
-    <row r="449" ht="14.25" customHeight="1"/>
-    <row r="450" ht="14.25" customHeight="1"/>
-    <row r="451" ht="14.25" customHeight="1"/>
-    <row r="452" ht="14.25" customHeight="1"/>
-    <row r="453" ht="14.25" customHeight="1"/>
-    <row r="454" ht="14.25" customHeight="1"/>
-    <row r="455" ht="14.25" customHeight="1"/>
-    <row r="456" ht="14.25" customHeight="1"/>
-    <row r="457" ht="14.25" customHeight="1"/>
-    <row r="458" ht="14.25" customHeight="1"/>
-    <row r="459" ht="14.25" customHeight="1"/>
-    <row r="460" ht="14.25" customHeight="1"/>
-    <row r="461" ht="14.25" customHeight="1"/>
-    <row r="462" ht="14.25" customHeight="1"/>
-    <row r="463" ht="14.25" customHeight="1"/>
-    <row r="464" ht="14.25" customHeight="1"/>
-    <row r="465" ht="14.25" customHeight="1"/>
-    <row r="466" ht="14.25" customHeight="1"/>
-    <row r="467" ht="14.25" customHeight="1"/>
-    <row r="468" ht="14.25" customHeight="1"/>
-    <row r="469" ht="14.25" customHeight="1"/>
-    <row r="470" ht="14.25" customHeight="1"/>
-    <row r="471" ht="14.25" customHeight="1"/>
-    <row r="472" ht="14.25" customHeight="1"/>
-    <row r="473" ht="14.25" customHeight="1"/>
-    <row r="474" ht="14.25" customHeight="1"/>
-    <row r="475" ht="14.25" customHeight="1"/>
-    <row r="476" ht="14.25" customHeight="1"/>
-    <row r="477" ht="14.25" customHeight="1"/>
-    <row r="478" ht="14.25" customHeight="1"/>
-    <row r="479" ht="14.25" customHeight="1"/>
-    <row r="480" ht="14.25" customHeight="1"/>
-    <row r="481" ht="14.25" customHeight="1"/>
-    <row r="482" ht="14.25" customHeight="1"/>
-    <row r="483" ht="14.25" customHeight="1"/>
-    <row r="484" ht="14.25" customHeight="1"/>
-    <row r="485" ht="14.25" customHeight="1"/>
-    <row r="486" ht="14.25" customHeight="1"/>
-    <row r="487" ht="14.25" customHeight="1"/>
-    <row r="488" ht="14.25" customHeight="1"/>
-    <row r="489" ht="14.25" customHeight="1"/>
-    <row r="490" ht="14.25" customHeight="1"/>
-    <row r="491" ht="14.25" customHeight="1"/>
-    <row r="492" ht="14.25" customHeight="1"/>
-    <row r="493" ht="14.25" customHeight="1"/>
-    <row r="494" ht="14.25" customHeight="1"/>
-    <row r="495" ht="14.25" customHeight="1"/>
-    <row r="496" ht="14.25" customHeight="1"/>
-    <row r="497" ht="14.25" customHeight="1"/>
-    <row r="498" ht="14.25" customHeight="1"/>
-    <row r="499" ht="14.25" customHeight="1"/>
-    <row r="500" ht="14.25" customHeight="1"/>
-    <row r="501" ht="14.25" customHeight="1"/>
-    <row r="502" ht="14.25" customHeight="1"/>
-    <row r="503" ht="14.25" customHeight="1"/>
-    <row r="504" ht="14.25" customHeight="1"/>
-    <row r="505" ht="14.25" customHeight="1"/>
-    <row r="506" ht="14.25" customHeight="1"/>
-    <row r="507" ht="14.25" customHeight="1"/>
-    <row r="508" ht="14.25" customHeight="1"/>
-    <row r="509" ht="14.25" customHeight="1"/>
-    <row r="510" ht="14.25" customHeight="1"/>
-    <row r="511" ht="14.25" customHeight="1"/>
-    <row r="512" ht="14.25" customHeight="1"/>
-    <row r="513" ht="14.25" customHeight="1"/>
-    <row r="514" ht="14.25" customHeight="1"/>
-    <row r="515" ht="14.25" customHeight="1"/>
-    <row r="516" ht="14.25" customHeight="1"/>
-    <row r="517" ht="14.25" customHeight="1"/>
-    <row r="518" ht="14.25" customHeight="1"/>
-    <row r="519" ht="14.25" customHeight="1"/>
-    <row r="520" ht="14.25" customHeight="1"/>
-    <row r="521" ht="14.25" customHeight="1"/>
-    <row r="522" ht="14.25" customHeight="1"/>
-    <row r="523" ht="14.25" customHeight="1"/>
-    <row r="524" ht="14.25" customHeight="1"/>
-    <row r="525" ht="14.25" customHeight="1"/>
-    <row r="526" ht="14.25" customHeight="1"/>
-    <row r="527" ht="14.25" customHeight="1"/>
-    <row r="528" ht="14.25" customHeight="1"/>
-    <row r="529" ht="14.25" customHeight="1"/>
-    <row r="530" ht="14.25" customHeight="1"/>
-    <row r="531" ht="14.25" customHeight="1"/>
-    <row r="532" ht="14.25" customHeight="1"/>
-    <row r="533" ht="14.25" customHeight="1"/>
-    <row r="534" ht="14.25" customHeight="1"/>
-    <row r="535" ht="14.25" customHeight="1"/>
-    <row r="536" ht="14.25" customHeight="1"/>
-    <row r="537" ht="14.25" customHeight="1"/>
-    <row r="538" ht="14.25" customHeight="1"/>
-    <row r="539" ht="14.25" customHeight="1"/>
-    <row r="540" ht="14.25" customHeight="1"/>
-    <row r="541" ht="14.25" customHeight="1"/>
-    <row r="542" ht="14.25" customHeight="1"/>
-    <row r="543" ht="14.25" customHeight="1"/>
-    <row r="544" ht="14.25" customHeight="1"/>
-    <row r="545" ht="14.25" customHeight="1"/>
-    <row r="546" ht="14.25" customHeight="1"/>
-    <row r="547" ht="14.25" customHeight="1"/>
-    <row r="548" ht="14.25" customHeight="1"/>
-    <row r="549" ht="14.25" customHeight="1"/>
-    <row r="550" ht="14.25" customHeight="1"/>
-    <row r="551" ht="14.25" customHeight="1"/>
-    <row r="552" ht="14.25" customHeight="1"/>
-    <row r="553" ht="14.25" customHeight="1"/>
-    <row r="554" ht="14.25" customHeight="1"/>
-    <row r="555" ht="14.25" customHeight="1"/>
-    <row r="556" ht="14.25" customHeight="1"/>
-    <row r="557" ht="14.25" customHeight="1"/>
-    <row r="558" ht="14.25" customHeight="1"/>
-    <row r="559" ht="14.25" customHeight="1"/>
-    <row r="560" ht="14.25" customHeight="1"/>
-    <row r="561" ht="14.25" customHeight="1"/>
-    <row r="562" ht="14.25" customHeight="1"/>
-    <row r="563" ht="14.25" customHeight="1"/>
-    <row r="564" ht="14.25" customHeight="1"/>
-    <row r="565" ht="14.25" customHeight="1"/>
-    <row r="566" ht="14.25" customHeight="1"/>
-    <row r="567" ht="14.25" customHeight="1"/>
-    <row r="568" ht="14.25" customHeight="1"/>
-    <row r="569" ht="14.25" customHeight="1"/>
-    <row r="570" ht="14.25" customHeight="1"/>
-    <row r="571" ht="14.25" customHeight="1"/>
-    <row r="572" ht="14.25" customHeight="1"/>
-    <row r="573" ht="14.25" customHeight="1"/>
-    <row r="574" ht="14.25" customHeight="1"/>
-    <row r="575" ht="14.25" customHeight="1"/>
-    <row r="576" ht="14.25" customHeight="1"/>
-    <row r="577" ht="14.25" customHeight="1"/>
-    <row r="578" ht="14.25" customHeight="1"/>
-    <row r="579" ht="14.25" customHeight="1"/>
-    <row r="580" ht="14.25" customHeight="1"/>
-    <row r="581" ht="14.25" customHeight="1"/>
-    <row r="582" ht="14.25" customHeight="1"/>
-    <row r="583" ht="14.25" customHeight="1"/>
-    <row r="584" ht="14.25" customHeight="1"/>
-    <row r="585" ht="14.25" customHeight="1"/>
-    <row r="586" ht="14.25" customHeight="1"/>
-    <row r="587" ht="14.25" customHeight="1"/>
-    <row r="588" ht="14.25" customHeight="1"/>
-    <row r="589" ht="14.25" customHeight="1"/>
-    <row r="590" ht="14.25" customHeight="1"/>
-    <row r="591" ht="14.25" customHeight="1"/>
-    <row r="592" ht="14.25" customHeight="1"/>
-    <row r="593" ht="14.25" customHeight="1"/>
-    <row r="594" ht="14.25" customHeight="1"/>
-    <row r="595" ht="14.25" customHeight="1"/>
-    <row r="596" ht="14.25" customHeight="1"/>
-    <row r="597" ht="14.25" customHeight="1"/>
-    <row r="598" ht="14.25" customHeight="1"/>
-    <row r="599" ht="14.25" customHeight="1"/>
-    <row r="600" ht="14.25" customHeight="1"/>
-    <row r="601" ht="14.25" customHeight="1"/>
-    <row r="602" ht="14.25" customHeight="1"/>
-    <row r="603" ht="14.25" customHeight="1"/>
-    <row r="604" ht="14.25" customHeight="1"/>
-    <row r="605" ht="14.25" customHeight="1"/>
-    <row r="606" ht="14.25" customHeight="1"/>
-    <row r="607" ht="14.25" customHeight="1"/>
-    <row r="608" ht="14.25" customHeight="1"/>
-    <row r="609" ht="14.25" customHeight="1"/>
-    <row r="610" ht="14.25" customHeight="1"/>
-    <row r="611" ht="14.25" customHeight="1"/>
-    <row r="612" ht="14.25" customHeight="1"/>
-    <row r="613" ht="14.25" customHeight="1"/>
-    <row r="614" ht="14.25" customHeight="1"/>
-    <row r="615" ht="14.25" customHeight="1"/>
-    <row r="616" ht="14.25" customHeight="1"/>
-    <row r="617" ht="14.25" customHeight="1"/>
-    <row r="618" ht="14.25" customHeight="1"/>
-    <row r="619" ht="14.25" customHeight="1"/>
-    <row r="620" ht="14.25" customHeight="1"/>
-    <row r="621" ht="14.25" customHeight="1"/>
-    <row r="622" ht="14.25" customHeight="1"/>
-    <row r="623" ht="14.25" customHeight="1"/>
-    <row r="624" ht="14.25" customHeight="1"/>
-    <row r="625" ht="14.25" customHeight="1"/>
-    <row r="626" ht="14.25" customHeight="1"/>
-    <row r="627" ht="14.25" customHeight="1"/>
-    <row r="628" ht="14.25" customHeight="1"/>
-    <row r="629" ht="14.25" customHeight="1"/>
-    <row r="630" ht="14.25" customHeight="1"/>
-    <row r="631" ht="14.25" customHeight="1"/>
-    <row r="632" ht="14.25" customHeight="1"/>
-    <row r="633" ht="14.25" customHeight="1"/>
-    <row r="634" ht="14.25" customHeight="1"/>
-    <row r="635" ht="14.25" customHeight="1"/>
-    <row r="636" ht="14.25" customHeight="1"/>
-    <row r="637" ht="14.25" customHeight="1"/>
-    <row r="638" ht="14.25" customHeight="1"/>
-    <row r="639" ht="14.25" customHeight="1"/>
-    <row r="640" ht="14.25" customHeight="1"/>
-    <row r="641" ht="14.25" customHeight="1"/>
-    <row r="642" ht="14.25" customHeight="1"/>
-    <row r="643" ht="14.25" customHeight="1"/>
-    <row r="644" ht="14.25" customHeight="1"/>
-    <row r="645" ht="14.25" customHeight="1"/>
-    <row r="646" ht="14.25" customHeight="1"/>
-    <row r="647" ht="14.25" customHeight="1"/>
-    <row r="648" ht="14.25" customHeight="1"/>
-    <row r="649" ht="14.25" customHeight="1"/>
-    <row r="650" ht="14.25" customHeight="1"/>
-    <row r="651" ht="14.25" customHeight="1"/>
-    <row r="652" ht="14.25" customHeight="1"/>
-    <row r="653" ht="14.25" customHeight="1"/>
-    <row r="654" ht="14.25" customHeight="1"/>
-    <row r="655" ht="14.25" customHeight="1"/>
-    <row r="656" ht="14.25" customHeight="1"/>
-    <row r="657" ht="14.25" customHeight="1"/>
-    <row r="658" ht="14.25" customHeight="1"/>
-    <row r="659" ht="14.25" customHeight="1"/>
-    <row r="660" ht="14.25" customHeight="1"/>
-    <row r="661" ht="14.25" customHeight="1"/>
-    <row r="662" ht="14.25" customHeight="1"/>
-    <row r="663" ht="14.25" customHeight="1"/>
-    <row r="664" ht="14.25" customHeight="1"/>
-    <row r="665" ht="14.25" customHeight="1"/>
-    <row r="666" ht="14.25" customHeight="1"/>
-    <row r="667" ht="14.25" customHeight="1"/>
-    <row r="668" ht="14.25" customHeight="1"/>
-    <row r="669" ht="14.25" customHeight="1"/>
-    <row r="670" ht="14.25" customHeight="1"/>
-    <row r="671" ht="14.25" customHeight="1"/>
-    <row r="672" ht="14.25" customHeight="1"/>
-    <row r="673" ht="14.25" customHeight="1"/>
-    <row r="674" ht="14.25" customHeight="1"/>
-    <row r="675" ht="14.25" customHeight="1"/>
-    <row r="676" ht="14.25" customHeight="1"/>
-    <row r="677" ht="14.25" customHeight="1"/>
-    <row r="678" ht="14.25" customHeight="1"/>
-    <row r="679" ht="14.25" customHeight="1"/>
-    <row r="680" ht="14.25" customHeight="1"/>
-    <row r="681" ht="14.25" customHeight="1"/>
-    <row r="682" ht="14.25" customHeight="1"/>
-    <row r="683" ht="14.25" customHeight="1"/>
-    <row r="684" ht="14.25" customHeight="1"/>
-    <row r="685" ht="14.25" customHeight="1"/>
-    <row r="686" ht="14.25" customHeight="1"/>
-    <row r="687" ht="14.25" customHeight="1"/>
-    <row r="688" ht="14.25" customHeight="1"/>
-    <row r="689" ht="14.25" customHeight="1"/>
-    <row r="690" ht="14.25" customHeight="1"/>
-    <row r="691" ht="14.25" customHeight="1"/>
-    <row r="692" ht="14.25" customHeight="1"/>
-    <row r="693" ht="14.25" customHeight="1"/>
-    <row r="694" ht="14.25" customHeight="1"/>
-    <row r="695" ht="14.25" customHeight="1"/>
-    <row r="696" ht="14.25" customHeight="1"/>
-    <row r="697" ht="14.25" customHeight="1"/>
-    <row r="698" ht="14.25" customHeight="1"/>
-    <row r="699" ht="14.25" customHeight="1"/>
-    <row r="700" ht="14.25" customHeight="1"/>
-    <row r="701" ht="14.25" customHeight="1"/>
-    <row r="702" ht="14.25" customHeight="1"/>
-    <row r="703" ht="14.25" customHeight="1"/>
-    <row r="704" ht="14.25" customHeight="1"/>
-    <row r="705" ht="14.25" customHeight="1"/>
-    <row r="706" ht="14.25" customHeight="1"/>
-    <row r="707" ht="14.25" customHeight="1"/>
-    <row r="708" ht="14.25" customHeight="1"/>
-    <row r="709" ht="14.25" customHeight="1"/>
-    <row r="710" ht="14.25" customHeight="1"/>
-    <row r="711" ht="14.25" customHeight="1"/>
-    <row r="712" ht="14.25" customHeight="1"/>
-    <row r="713" ht="14.25" customHeight="1"/>
-    <row r="714" ht="14.25" customHeight="1"/>
-    <row r="715" ht="14.25" customHeight="1"/>
-    <row r="716" ht="14.25" customHeight="1"/>
-    <row r="717" ht="14.25" customHeight="1"/>
-    <row r="718" ht="14.25" customHeight="1"/>
-    <row r="719" ht="14.25" customHeight="1"/>
-    <row r="720" ht="14.25" customHeight="1"/>
-    <row r="721" ht="14.25" customHeight="1"/>
-    <row r="722" ht="14.25" customHeight="1"/>
-    <row r="723" ht="14.25" customHeight="1"/>
-    <row r="724" ht="14.25" customHeight="1"/>
-    <row r="725" ht="14.25" customHeight="1"/>
-    <row r="726" ht="14.25" customHeight="1"/>
-    <row r="727" ht="14.25" customHeight="1"/>
-    <row r="728" ht="14.25" customHeight="1"/>
-    <row r="729" ht="14.25" customHeight="1"/>
-    <row r="730" ht="14.25" customHeight="1"/>
-    <row r="731" ht="14.25" customHeight="1"/>
-    <row r="732" ht="14.25" customHeight="1"/>
-    <row r="733" ht="14.25" customHeight="1"/>
-    <row r="734" ht="14.25" customHeight="1"/>
-    <row r="735" ht="14.25" customHeight="1"/>
-    <row r="736" ht="14.25" customHeight="1"/>
-    <row r="737" ht="14.25" customHeight="1"/>
-    <row r="738" ht="14.25" customHeight="1"/>
-    <row r="739" ht="14.25" customHeight="1"/>
-    <row r="740" ht="14.25" customHeight="1"/>
-    <row r="741" ht="14.25" customHeight="1"/>
-    <row r="742" ht="14.25" customHeight="1"/>
-    <row r="743" ht="14.25" customHeight="1"/>
-    <row r="744" ht="14.25" customHeight="1"/>
-    <row r="745" ht="14.25" customHeight="1"/>
-    <row r="746" ht="14.25" customHeight="1"/>
-    <row r="747" ht="14.25" customHeight="1"/>
-    <row r="748" ht="14.25" customHeight="1"/>
-    <row r="749" ht="14.25" customHeight="1"/>
-    <row r="750" ht="14.25" customHeight="1"/>
-    <row r="751" ht="14.25" customHeight="1"/>
-    <row r="752" ht="14.25" customHeight="1"/>
-    <row r="753" ht="14.25" customHeight="1"/>
-    <row r="754" ht="14.25" customHeight="1"/>
-    <row r="755" ht="14.25" customHeight="1"/>
-    <row r="756" ht="14.25" customHeight="1"/>
-    <row r="757" ht="14.25" customHeight="1"/>
-    <row r="758" ht="14.25" customHeight="1"/>
-    <row r="759" ht="14.25" customHeight="1"/>
-    <row r="760" ht="14.25" customHeight="1"/>
-    <row r="761" ht="14.25" customHeight="1"/>
-    <row r="762" ht="14.25" customHeight="1"/>
-    <row r="763" ht="14.25" customHeight="1"/>
-    <row r="764" ht="14.25" customHeight="1"/>
-    <row r="765" ht="14.25" customHeight="1"/>
-    <row r="766" ht="14.25" customHeight="1"/>
-    <row r="767" ht="14.25" customHeight="1"/>
-    <row r="768" ht="14.25" customHeight="1"/>
-    <row r="769" ht="14.25" customHeight="1"/>
-    <row r="770" ht="14.25" customHeight="1"/>
-    <row r="771" ht="14.25" customHeight="1"/>
-    <row r="772" ht="14.25" customHeight="1"/>
-    <row r="773" ht="14.25" customHeight="1"/>
-    <row r="774" ht="14.25" customHeight="1"/>
-    <row r="775" ht="14.25" customHeight="1"/>
-    <row r="776" ht="14.25" customHeight="1"/>
-    <row r="777" ht="14.25" customHeight="1"/>
-    <row r="778" ht="14.25" customHeight="1"/>
-    <row r="779" ht="14.25" customHeight="1"/>
-    <row r="780" ht="14.25" customHeight="1"/>
-    <row r="781" ht="14.25" customHeight="1"/>
-    <row r="782" ht="14.25" customHeight="1"/>
-    <row r="783" ht="14.25" customHeight="1"/>
-    <row r="784" ht="14.25" customHeight="1"/>
-    <row r="785" ht="14.25" customHeight="1"/>
-    <row r="786" ht="14.25" customHeight="1"/>
-    <row r="787" ht="14.25" customHeight="1"/>
-    <row r="788" ht="14.25" customHeight="1"/>
-    <row r="789" ht="14.25" customHeight="1"/>
-    <row r="790" ht="14.25" customHeight="1"/>
-    <row r="791" ht="14.25" customHeight="1"/>
-    <row r="792" ht="14.25" customHeight="1"/>
-    <row r="793" ht="14.25" customHeight="1"/>
-    <row r="794" ht="14.25" customHeight="1"/>
-    <row r="795" ht="14.25" customHeight="1"/>
-    <row r="796" ht="14.25" customHeight="1"/>
-    <row r="797" ht="14.25" customHeight="1"/>
-    <row r="798" ht="14.25" customHeight="1"/>
-    <row r="799" ht="14.25" customHeight="1"/>
-    <row r="800" ht="14.25" customHeight="1"/>
-    <row r="801" ht="14.25" customHeight="1"/>
-    <row r="802" ht="14.25" customHeight="1"/>
-    <row r="803" ht="14.25" customHeight="1"/>
-    <row r="804" ht="14.25" customHeight="1"/>
-    <row r="805" ht="14.25" customHeight="1"/>
-    <row r="806" ht="14.25" customHeight="1"/>
-    <row r="807" ht="14.25" customHeight="1"/>
-    <row r="808" ht="14.25" customHeight="1"/>
-    <row r="809" ht="14.25" customHeight="1"/>
-    <row r="810" ht="14.25" customHeight="1"/>
-    <row r="811" ht="14.25" customHeight="1"/>
-    <row r="812" ht="14.25" customHeight="1"/>
-    <row r="813" ht="14.25" customHeight="1"/>
-    <row r="814" ht="14.25" customHeight="1"/>
-    <row r="815" ht="14.25" customHeight="1"/>
-    <row r="816" ht="14.25" customHeight="1"/>
-    <row r="817" ht="14.25" customHeight="1"/>
-    <row r="818" ht="14.25" customHeight="1"/>
-    <row r="819" ht="14.25" customHeight="1"/>
-    <row r="820" ht="14.25" customHeight="1"/>
-    <row r="821" ht="14.25" customHeight="1"/>
-    <row r="822" ht="14.25" customHeight="1"/>
-    <row r="823" ht="14.25" customHeight="1"/>
-    <row r="824" ht="14.25" customHeight="1"/>
-    <row r="825" ht="14.25" customHeight="1"/>
-    <row r="826" ht="14.25" customHeight="1"/>
-    <row r="827" ht="14.25" customHeight="1"/>
-    <row r="828" ht="14.25" customHeight="1"/>
-    <row r="829" ht="14.25" customHeight="1"/>
-    <row r="830" ht="14.25" customHeight="1"/>
-    <row r="831" ht="14.25" customHeight="1"/>
-    <row r="832" ht="14.25" customHeight="1"/>
-    <row r="833" ht="14.25" customHeight="1"/>
-    <row r="834" ht="14.25" customHeight="1"/>
-    <row r="835" ht="14.25" customHeight="1"/>
-    <row r="836" ht="14.25" customHeight="1"/>
-    <row r="837" ht="14.25" customHeight="1"/>
-    <row r="838" ht="14.25" customHeight="1"/>
-    <row r="839" ht="14.25" customHeight="1"/>
-    <row r="840" ht="14.25" customHeight="1"/>
-    <row r="841" ht="14.25" customHeight="1"/>
-    <row r="842" ht="14.25" customHeight="1"/>
-    <row r="843" ht="14.25" customHeight="1"/>
-    <row r="844" ht="14.25" customHeight="1"/>
-    <row r="845" ht="14.25" customHeight="1"/>
-    <row r="846" ht="14.25" customHeight="1"/>
-    <row r="847" ht="14.25" customHeight="1"/>
-    <row r="848" ht="14.25" customHeight="1"/>
-    <row r="849" ht="14.25" customHeight="1"/>
-    <row r="850" ht="14.25" customHeight="1"/>
-    <row r="851" ht="14.25" customHeight="1"/>
-    <row r="852" ht="14.25" customHeight="1"/>
-    <row r="853" ht="14.25" customHeight="1"/>
-    <row r="854" ht="14.25" customHeight="1"/>
-    <row r="855" ht="14.25" customHeight="1"/>
-    <row r="856" ht="14.25" customHeight="1"/>
-    <row r="857" ht="14.25" customHeight="1"/>
-    <row r="858" ht="14.25" customHeight="1"/>
-    <row r="859" ht="14.25" customHeight="1"/>
-    <row r="860" ht="14.25" customHeight="1"/>
-    <row r="861" ht="14.25" customHeight="1"/>
-    <row r="862" ht="14.25" customHeight="1"/>
-    <row r="863" ht="14.25" customHeight="1"/>
-    <row r="864" ht="14.25" customHeight="1"/>
-    <row r="865" ht="14.25" customHeight="1"/>
-    <row r="866" ht="14.25" customHeight="1"/>
-    <row r="867" ht="14.25" customHeight="1"/>
-    <row r="868" ht="14.25" customHeight="1"/>
-    <row r="869" ht="14.25" customHeight="1"/>
-    <row r="870" ht="14.25" customHeight="1"/>
-    <row r="871" ht="14.25" customHeight="1"/>
-    <row r="872" ht="14.25" customHeight="1"/>
-    <row r="873" ht="14.25" customHeight="1"/>
-    <row r="874" ht="14.25" customHeight="1"/>
-    <row r="875" ht="14.25" customHeight="1"/>
-    <row r="876" ht="14.25" customHeight="1"/>
-    <row r="877" ht="14.25" customHeight="1"/>
-    <row r="878" ht="14.25" customHeight="1"/>
-    <row r="879" ht="14.25" customHeight="1"/>
-    <row r="880" ht="14.25" customHeight="1"/>
-    <row r="881" ht="14.25" customHeight="1"/>
-    <row r="882" ht="14.25" customHeight="1"/>
-    <row r="883" ht="14.25" customHeight="1"/>
-    <row r="884" ht="14.25" customHeight="1"/>
-    <row r="885" ht="14.25" customHeight="1"/>
-    <row r="886" ht="14.25" customHeight="1"/>
-    <row r="887" ht="14.25" customHeight="1"/>
-    <row r="888" ht="14.25" customHeight="1"/>
-    <row r="889" ht="14.25" customHeight="1"/>
-    <row r="890" ht="14.25" customHeight="1"/>
-    <row r="891" ht="14.25" customHeight="1"/>
-    <row r="892" ht="14.25" customHeight="1"/>
-    <row r="893" ht="14.25" customHeight="1"/>
-    <row r="894" ht="14.25" customHeight="1"/>
-    <row r="895" ht="14.25" customHeight="1"/>
-    <row r="896" ht="14.25" customHeight="1"/>
-    <row r="897" ht="14.25" customHeight="1"/>
-    <row r="898" ht="14.25" customHeight="1"/>
-    <row r="899" ht="14.25" customHeight="1"/>
-    <row r="900" ht="14.25" customHeight="1"/>
-    <row r="901" ht="14.25" customHeight="1"/>
-    <row r="902" ht="14.25" customHeight="1"/>
-    <row r="903" ht="14.25" customHeight="1"/>
-    <row r="904" ht="14.25" customHeight="1"/>
-    <row r="905" ht="14.25" customHeight="1"/>
-    <row r="906" ht="14.25" customHeight="1"/>
-    <row r="907" ht="14.25" customHeight="1"/>
-    <row r="908" ht="14.25" customHeight="1"/>
-    <row r="909" ht="14.25" customHeight="1"/>
-    <row r="910" ht="14.25" customHeight="1"/>
-    <row r="911" ht="14.25" customHeight="1"/>
-    <row r="912" ht="14.25" customHeight="1"/>
-    <row r="913" ht="14.25" customHeight="1"/>
-    <row r="914" ht="14.25" customHeight="1"/>
-    <row r="915" ht="14.25" customHeight="1"/>
-    <row r="916" ht="14.25" customHeight="1"/>
-    <row r="917" ht="14.25" customHeight="1"/>
-    <row r="918" ht="14.25" customHeight="1"/>
-    <row r="919" ht="14.25" customHeight="1"/>
-    <row r="920" ht="14.25" customHeight="1"/>
-    <row r="921" ht="14.25" customHeight="1"/>
-    <row r="922" ht="14.25" customHeight="1"/>
-    <row r="923" ht="14.25" customHeight="1"/>
-    <row r="924" ht="14.25" customHeight="1"/>
-    <row r="925" ht="14.25" customHeight="1"/>
-    <row r="926" ht="14.25" customHeight="1"/>
-    <row r="927" ht="14.25" customHeight="1"/>
-    <row r="928" ht="14.25" customHeight="1"/>
-    <row r="929" ht="14.25" customHeight="1"/>
-    <row r="930" ht="14.25" customHeight="1"/>
-    <row r="931" ht="14.25" customHeight="1"/>
-    <row r="932" ht="14.25" customHeight="1"/>
-    <row r="933" ht="14.25" customHeight="1"/>
-    <row r="934" ht="14.25" customHeight="1"/>
-    <row r="935" ht="14.25" customHeight="1"/>
-    <row r="936" ht="14.25" customHeight="1"/>
-    <row r="937" ht="14.25" customHeight="1"/>
-    <row r="938" ht="14.25" customHeight="1"/>
-    <row r="939" ht="14.25" customHeight="1"/>
-    <row r="940" ht="14.25" customHeight="1"/>
-    <row r="941" ht="14.25" customHeight="1"/>
-    <row r="942" ht="14.25" customHeight="1"/>
-    <row r="943" ht="14.25" customHeight="1"/>
-    <row r="944" ht="14.25" customHeight="1"/>
-    <row r="945" ht="14.25" customHeight="1"/>
-    <row r="946" ht="14.25" customHeight="1"/>
-    <row r="947" ht="14.25" customHeight="1"/>
-    <row r="948" ht="14.25" customHeight="1"/>
-    <row r="949" ht="14.25" customHeight="1"/>
-    <row r="950" ht="14.25" customHeight="1"/>
-    <row r="951" ht="14.25" customHeight="1"/>
-    <row r="952" ht="14.25" customHeight="1"/>
-    <row r="953" ht="14.25" customHeight="1"/>
-    <row r="954" ht="14.25" customHeight="1"/>
-    <row r="955" ht="14.25" customHeight="1"/>
-    <row r="956" ht="14.25" customHeight="1"/>
-    <row r="957" ht="14.25" customHeight="1"/>
-    <row r="958" ht="14.25" customHeight="1"/>
-    <row r="959" ht="14.25" customHeight="1"/>
-    <row r="960" ht="14.25" customHeight="1"/>
-    <row r="961" ht="14.25" customHeight="1"/>
-    <row r="962" ht="14.25" customHeight="1"/>
-    <row r="963" ht="14.25" customHeight="1"/>
-    <row r="964" ht="14.25" customHeight="1"/>
-    <row r="965" ht="14.25" customHeight="1"/>
-    <row r="966" ht="14.25" customHeight="1"/>
-    <row r="967" ht="14.25" customHeight="1"/>
-    <row r="968" ht="14.25" customHeight="1"/>
-    <row r="969" ht="14.25" customHeight="1"/>
-    <row r="970" ht="14.25" customHeight="1"/>
-    <row r="971" ht="14.25" customHeight="1"/>
-    <row r="972" ht="14.25" customHeight="1"/>
-    <row r="973" ht="14.25" customHeight="1"/>
-    <row r="974" ht="14.25" customHeight="1"/>
-    <row r="975" ht="14.25" customHeight="1"/>
-    <row r="976" ht="14.25" customHeight="1"/>
-    <row r="977" ht="14.25" customHeight="1"/>
-    <row r="978" ht="14.25" customHeight="1"/>
-    <row r="979" ht="14.25" customHeight="1"/>
-    <row r="980" ht="14.25" customHeight="1"/>
-    <row r="981" ht="14.25" customHeight="1"/>
-    <row r="982" ht="14.25" customHeight="1"/>
-    <row r="983" ht="14.25" customHeight="1"/>
-    <row r="984" ht="14.25" customHeight="1"/>
-    <row r="985" ht="14.25" customHeight="1"/>
-    <row r="986" ht="14.25" customHeight="1"/>
-    <row r="987" ht="14.25" customHeight="1"/>
-    <row r="988" ht="14.25" customHeight="1"/>
-    <row r="989" ht="14.25" customHeight="1"/>
-    <row r="990" ht="14.25" customHeight="1"/>
-    <row r="991" ht="14.25" customHeight="1"/>
-    <row r="992" ht="14.25" customHeight="1"/>
-    <row r="993" ht="14.25" customHeight="1"/>
-    <row r="994" ht="14.25" customHeight="1"/>
-    <row r="995" ht="14.25" customHeight="1"/>
-    <row r="996" ht="14.25" customHeight="1"/>
-    <row r="997" ht="14.25" customHeight="1"/>
-    <row r="998" ht="14.25" customHeight="1"/>
-    <row r="999" ht="14.25" customHeight="1"/>
-    <row r="1000" ht="14.25" customHeight="1"/>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="B3:F3"/>
-  </mergeCells>
-  <printOptions/>
-  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
-  <pageSetup orientation="landscape"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>